<commit_message>
Updating COC's and Download Links, replacing old Test Quote with V4
</commit_message>
<xml_diff>
--- a/src/Assets/files/COC's/ALS COC Jackson PFAS Solids & Liquids.xlsx
+++ b/src/Assets/files/COC's/ALS COC Jackson PFAS Solids & Liquids.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://purenvau-my.sharepoint.com/personal/rpope_purenv_au/Documents/Desktop/Projects/InterDepartmental/Environmental Monitoring Spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://purenvau.sharepoint.com/sites/Westrex/Shared Documents/General/1. WestRex (Jackson)/Site Testing/ALS Information, COC's, and Quotes/COC Blanks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{586D3D75-B624-4776-919F-9C3B3A89AAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6583BD06-E48F-4EF3-B96C-439FE61C4B64}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="8_{586D3D75-B624-4776-919F-9C3B3A89AAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1D7A36E-433D-4346-AFC1-76BDC8E8A538}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D6F1A21B-16EA-4DE4-84E7-4FFDAAE173B9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D6F1A21B-16EA-4DE4-84E7-4FFDAAE173B9}"/>
   </bookViews>
   <sheets>
     <sheet name="ENFM 204.17" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="89">
   <si>
     <t>Mandatory Fields</t>
   </si>
@@ -829,33 +829,30 @@
     <t xml:space="preserve">ap.regional@purenv.au   kyip@purenv.au   dclaridge@purenv.au </t>
   </si>
   <si>
-    <t xml:space="preserve">hseq.qld@purenv.au
+    <t>-</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>PFAS Solid/Liquid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hseq.qldregional@purenv.au
 kyip@purenv.au
 dclaridge@purenv.au </t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>Sample X</t>
-  </si>
-  <si>
-    <t>PFAS Solid/Liquid</t>
-  </si>
-  <si>
-    <t>Sample Y</t>
-  </si>
-  <si>
-    <t>Table 8</t>
-  </si>
-  <si>
-    <t>Table 9</t>
+    <t>Table 8 EP231X Full Suite</t>
+  </si>
+  <si>
+    <t>Table 8 EP231X (TOP)</t>
+  </si>
+  <si>
+    <t>Table 9 EP231X (Leachate)</t>
+  </si>
+  <si>
+    <t>Table 9 EP231X (Solids)</t>
   </si>
 </sst>
 </file>
@@ -1821,6 +1818,444 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="31" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="35" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1938,282 +2373,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="35" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2225,168 +2384,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="31" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2766,7 +2763,7 @@
   <dimension ref="A1:AU33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="50" zoomScalePageLayoutView="106" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+      <selection activeCell="AW8" sqref="AW8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2788,107 +2785,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="168" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="106"/>
-      <c r="J1" s="107" t="s">
+      <c r="B1" s="169"/>
+      <c r="C1" s="169"/>
+      <c r="D1" s="169"/>
+      <c r="E1" s="169"/>
+      <c r="F1" s="169"/>
+      <c r="G1" s="169"/>
+      <c r="H1" s="169"/>
+      <c r="I1" s="170"/>
+      <c r="J1" s="171" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="108"/>
-      <c r="L1" s="108"/>
-      <c r="M1" s="108"/>
-      <c r="N1" s="108"/>
-      <c r="O1" s="108"/>
-      <c r="P1" s="108"/>
-      <c r="Q1" s="108"/>
-      <c r="R1" s="108"/>
-      <c r="S1" s="108"/>
-      <c r="T1" s="108"/>
-      <c r="U1" s="108"/>
-      <c r="V1" s="108"/>
-      <c r="W1" s="108"/>
-      <c r="X1" s="108"/>
-      <c r="Y1" s="108"/>
-      <c r="Z1" s="108"/>
-      <c r="AA1" s="108"/>
-      <c r="AB1" s="108"/>
-      <c r="AC1" s="108"/>
-      <c r="AD1" s="108"/>
-      <c r="AE1" s="109"/>
-      <c r="AF1" s="110" t="s">
+      <c r="K1" s="172"/>
+      <c r="L1" s="172"/>
+      <c r="M1" s="172"/>
+      <c r="N1" s="172"/>
+      <c r="O1" s="172"/>
+      <c r="P1" s="172"/>
+      <c r="Q1" s="172"/>
+      <c r="R1" s="172"/>
+      <c r="S1" s="172"/>
+      <c r="T1" s="172"/>
+      <c r="U1" s="172"/>
+      <c r="V1" s="172"/>
+      <c r="W1" s="172"/>
+      <c r="X1" s="172"/>
+      <c r="Y1" s="172"/>
+      <c r="Z1" s="172"/>
+      <c r="AA1" s="172"/>
+      <c r="AB1" s="172"/>
+      <c r="AC1" s="172"/>
+      <c r="AD1" s="172"/>
+      <c r="AE1" s="173"/>
+      <c r="AF1" s="174" t="s">
         <v>73</v>
       </c>
-      <c r="AG1" s="111"/>
-      <c r="AH1" s="111"/>
-      <c r="AI1" s="111"/>
-      <c r="AJ1" s="114"/>
-      <c r="AK1" s="115"/>
-      <c r="AL1" s="115"/>
-      <c r="AM1" s="116"/>
+      <c r="AG1" s="175"/>
+      <c r="AH1" s="175"/>
+      <c r="AI1" s="175"/>
+      <c r="AJ1" s="178"/>
+      <c r="AK1" s="179"/>
+      <c r="AL1" s="179"/>
+      <c r="AM1" s="180"/>
       <c r="AO1" s="43"/>
       <c r="AP1" s="43"/>
       <c r="AQ1" s="43"/>
     </row>
     <row r="2" spans="1:47" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="123" t="s">
+      <c r="A2" s="187" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="124"/>
-      <c r="C2" s="228" t="s">
+      <c r="B2" s="188"/>
+      <c r="C2" s="101" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="228"/>
-      <c r="E2" s="228"/>
-      <c r="F2" s="228"/>
-      <c r="G2" s="228"/>
-      <c r="H2" s="228"/>
-      <c r="I2" s="228"/>
-      <c r="J2" s="125" t="s">
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="189" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="125"/>
-      <c r="L2" s="126" t="s">
+      <c r="K2" s="189"/>
+      <c r="L2" s="190" t="s">
         <v>74</v>
       </c>
-      <c r="M2" s="127"/>
-      <c r="N2" s="127"/>
-      <c r="O2" s="127"/>
-      <c r="P2" s="127"/>
-      <c r="Q2" s="127"/>
-      <c r="R2" s="127"/>
-      <c r="S2" s="127"/>
-      <c r="T2" s="127"/>
-      <c r="U2" s="127"/>
-      <c r="V2" s="128" t="s">
+      <c r="M2" s="191"/>
+      <c r="N2" s="191"/>
+      <c r="O2" s="191"/>
+      <c r="P2" s="191"/>
+      <c r="Q2" s="191"/>
+      <c r="R2" s="191"/>
+      <c r="S2" s="191"/>
+      <c r="T2" s="191"/>
+      <c r="U2" s="191"/>
+      <c r="V2" s="192" t="s">
         <v>4</v>
       </c>
-      <c r="W2" s="128"/>
-      <c r="X2" s="129" t="s">
+      <c r="W2" s="192"/>
+      <c r="X2" s="193" t="s">
         <v>75</v>
       </c>
-      <c r="Y2" s="129"/>
-      <c r="Z2" s="129"/>
-      <c r="AA2" s="129"/>
-      <c r="AB2" s="129"/>
-      <c r="AC2" s="129"/>
-      <c r="AD2" s="129"/>
-      <c r="AE2" s="130"/>
-      <c r="AF2" s="112"/>
-      <c r="AG2" s="113"/>
-      <c r="AH2" s="113"/>
-      <c r="AI2" s="113"/>
-      <c r="AJ2" s="117"/>
-      <c r="AK2" s="118"/>
-      <c r="AL2" s="118"/>
-      <c r="AM2" s="119"/>
+      <c r="Y2" s="193"/>
+      <c r="Z2" s="193"/>
+      <c r="AA2" s="193"/>
+      <c r="AB2" s="193"/>
+      <c r="AC2" s="193"/>
+      <c r="AD2" s="193"/>
+      <c r="AE2" s="194"/>
+      <c r="AF2" s="176"/>
+      <c r="AG2" s="177"/>
+      <c r="AH2" s="177"/>
+      <c r="AI2" s="177"/>
+      <c r="AJ2" s="181"/>
+      <c r="AK2" s="182"/>
+      <c r="AL2" s="182"/>
+      <c r="AM2" s="183"/>
       <c r="AO2" s="44" t="s">
         <v>5</v>
       </c>
@@ -2899,55 +2896,55 @@
       <c r="AR2" s="1"/>
     </row>
     <row r="3" spans="1:47" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="131" t="s">
+      <c r="A3" s="195" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="132"/>
-      <c r="C3" s="229" t="s">
+      <c r="B3" s="196"/>
+      <c r="C3" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="229"/>
-      <c r="E3" s="229"/>
-      <c r="F3" s="229"/>
-      <c r="G3" s="229"/>
-      <c r="H3" s="229"/>
-      <c r="I3" s="229"/>
-      <c r="J3" s="133" t="s">
+      <c r="D3" s="103"/>
+      <c r="E3" s="103"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="103"/>
+      <c r="H3" s="103"/>
+      <c r="I3" s="103"/>
+      <c r="J3" s="197" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="133"/>
-      <c r="L3" s="134"/>
-      <c r="M3" s="134"/>
-      <c r="N3" s="134"/>
-      <c r="O3" s="134"/>
-      <c r="P3" s="134"/>
-      <c r="Q3" s="134"/>
-      <c r="R3" s="134"/>
-      <c r="S3" s="134"/>
-      <c r="T3" s="134"/>
-      <c r="U3" s="134"/>
-      <c r="V3" s="135" t="s">
+      <c r="K3" s="197"/>
+      <c r="L3" s="198"/>
+      <c r="M3" s="198"/>
+      <c r="N3" s="198"/>
+      <c r="O3" s="198"/>
+      <c r="P3" s="198"/>
+      <c r="Q3" s="198"/>
+      <c r="R3" s="198"/>
+      <c r="S3" s="198"/>
+      <c r="T3" s="198"/>
+      <c r="U3" s="198"/>
+      <c r="V3" s="199" t="s">
         <v>9</v>
       </c>
-      <c r="W3" s="135"/>
-      <c r="X3" s="136"/>
-      <c r="Y3" s="136"/>
-      <c r="Z3" s="136"/>
-      <c r="AA3" s="136"/>
-      <c r="AB3" s="136"/>
-      <c r="AC3" s="136"/>
-      <c r="AD3" s="136"/>
-      <c r="AE3" s="137"/>
-      <c r="AF3" s="138" t="s">
+      <c r="W3" s="199"/>
+      <c r="X3" s="102"/>
+      <c r="Y3" s="102"/>
+      <c r="Z3" s="102"/>
+      <c r="AA3" s="102"/>
+      <c r="AB3" s="102"/>
+      <c r="AC3" s="102"/>
+      <c r="AD3" s="102"/>
+      <c r="AE3" s="200"/>
+      <c r="AF3" s="201" t="s">
         <v>10</v>
       </c>
-      <c r="AG3" s="139"/>
-      <c r="AH3" s="139"/>
-      <c r="AI3" s="139"/>
-      <c r="AJ3" s="117"/>
-      <c r="AK3" s="118"/>
-      <c r="AL3" s="118"/>
-      <c r="AM3" s="119"/>
+      <c r="AG3" s="202"/>
+      <c r="AH3" s="202"/>
+      <c r="AI3" s="202"/>
+      <c r="AJ3" s="181"/>
+      <c r="AK3" s="182"/>
+      <c r="AL3" s="182"/>
+      <c r="AM3" s="183"/>
       <c r="AO3" s="44"/>
       <c r="AP3" s="46" t="s">
         <v>11</v>
@@ -2956,161 +2953,161 @@
       <c r="AR3" s="1"/>
     </row>
     <row r="4" spans="1:47" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="140" t="s">
+      <c r="A4" s="203" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="135"/>
-      <c r="C4" s="136"/>
-      <c r="D4" s="136"/>
-      <c r="E4" s="136"/>
-      <c r="F4" s="136"/>
-      <c r="G4" s="136"/>
-      <c r="H4" s="136"/>
-      <c r="I4" s="135" t="s">
+      <c r="B4" s="199"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="102"/>
+      <c r="H4" s="102"/>
+      <c r="I4" s="199" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="135"/>
-      <c r="K4" s="135"/>
-      <c r="L4" s="136" t="s">
+      <c r="J4" s="199"/>
+      <c r="K4" s="199"/>
+      <c r="L4" s="102" t="s">
         <v>76</v>
       </c>
-      <c r="M4" s="136"/>
-      <c r="N4" s="136"/>
-      <c r="O4" s="136"/>
-      <c r="P4" s="136"/>
-      <c r="Q4" s="136"/>
-      <c r="R4" s="136"/>
-      <c r="S4" s="136"/>
-      <c r="T4" s="136"/>
-      <c r="U4" s="136"/>
-      <c r="V4" s="135" t="s">
+      <c r="M4" s="102"/>
+      <c r="N4" s="102"/>
+      <c r="O4" s="102"/>
+      <c r="P4" s="102"/>
+      <c r="Q4" s="102"/>
+      <c r="R4" s="102"/>
+      <c r="S4" s="102"/>
+      <c r="T4" s="102"/>
+      <c r="U4" s="102"/>
+      <c r="V4" s="199" t="s">
         <v>14</v>
       </c>
-      <c r="W4" s="135"/>
-      <c r="X4" s="136"/>
-      <c r="Y4" s="136"/>
-      <c r="Z4" s="136"/>
-      <c r="AA4" s="136"/>
-      <c r="AB4" s="136"/>
-      <c r="AC4" s="136"/>
-      <c r="AD4" s="136"/>
-      <c r="AE4" s="137"/>
-      <c r="AF4" s="141"/>
-      <c r="AG4" s="142"/>
-      <c r="AH4" s="142"/>
-      <c r="AI4" s="142"/>
-      <c r="AJ4" s="117"/>
-      <c r="AK4" s="118"/>
-      <c r="AL4" s="118"/>
-      <c r="AM4" s="119"/>
+      <c r="W4" s="199"/>
+      <c r="X4" s="102"/>
+      <c r="Y4" s="102"/>
+      <c r="Z4" s="102"/>
+      <c r="AA4" s="102"/>
+      <c r="AB4" s="102"/>
+      <c r="AC4" s="102"/>
+      <c r="AD4" s="102"/>
+      <c r="AE4" s="200"/>
+      <c r="AF4" s="204"/>
+      <c r="AG4" s="205"/>
+      <c r="AH4" s="205"/>
+      <c r="AI4" s="205"/>
+      <c r="AJ4" s="181"/>
+      <c r="AK4" s="182"/>
+      <c r="AL4" s="182"/>
+      <c r="AM4" s="183"/>
       <c r="AO4" s="44"/>
       <c r="AP4" s="44"/>
       <c r="AQ4" s="44"/>
       <c r="AR4" s="1"/>
     </row>
     <row r="5" spans="1:47" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="145" t="s">
+      <c r="A5" s="208" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="146"/>
-      <c r="C5" s="147" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" s="147"/>
-      <c r="E5" s="147"/>
-      <c r="F5" s="147"/>
-      <c r="G5" s="147"/>
-      <c r="H5" s="147"/>
-      <c r="I5" s="147"/>
-      <c r="J5" s="147"/>
-      <c r="K5" s="147"/>
-      <c r="L5" s="147"/>
-      <c r="M5" s="147"/>
-      <c r="N5" s="147"/>
-      <c r="O5" s="147"/>
-      <c r="P5" s="147"/>
-      <c r="Q5" s="147"/>
-      <c r="R5" s="147"/>
-      <c r="S5" s="147"/>
-      <c r="T5" s="147"/>
-      <c r="U5" s="147"/>
-      <c r="V5" s="146" t="s">
+      <c r="B5" s="209"/>
+      <c r="C5" s="210" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="210"/>
+      <c r="E5" s="210"/>
+      <c r="F5" s="210"/>
+      <c r="G5" s="210"/>
+      <c r="H5" s="210"/>
+      <c r="I5" s="210"/>
+      <c r="J5" s="210"/>
+      <c r="K5" s="210"/>
+      <c r="L5" s="210"/>
+      <c r="M5" s="210"/>
+      <c r="N5" s="210"/>
+      <c r="O5" s="210"/>
+      <c r="P5" s="210"/>
+      <c r="Q5" s="210"/>
+      <c r="R5" s="210"/>
+      <c r="S5" s="210"/>
+      <c r="T5" s="210"/>
+      <c r="U5" s="210"/>
+      <c r="V5" s="209" t="s">
         <v>16</v>
       </c>
-      <c r="W5" s="146"/>
-      <c r="X5" s="148" t="s">
+      <c r="W5" s="209"/>
+      <c r="X5" s="120" t="s">
         <v>77</v>
       </c>
-      <c r="Y5" s="148"/>
-      <c r="Z5" s="148"/>
-      <c r="AA5" s="148"/>
-      <c r="AB5" s="148"/>
-      <c r="AC5" s="148"/>
-      <c r="AD5" s="148"/>
-      <c r="AE5" s="149"/>
-      <c r="AF5" s="143"/>
-      <c r="AG5" s="144"/>
-      <c r="AH5" s="144"/>
-      <c r="AI5" s="144"/>
-      <c r="AJ5" s="120"/>
-      <c r="AK5" s="121"/>
-      <c r="AL5" s="121"/>
-      <c r="AM5" s="122"/>
+      <c r="Y5" s="120"/>
+      <c r="Z5" s="120"/>
+      <c r="AA5" s="120"/>
+      <c r="AB5" s="120"/>
+      <c r="AC5" s="120"/>
+      <c r="AD5" s="120"/>
+      <c r="AE5" s="121"/>
+      <c r="AF5" s="206"/>
+      <c r="AG5" s="207"/>
+      <c r="AH5" s="207"/>
+      <c r="AI5" s="207"/>
+      <c r="AJ5" s="184"/>
+      <c r="AK5" s="185"/>
+      <c r="AL5" s="185"/>
+      <c r="AM5" s="186"/>
       <c r="AO5" s="1"/>
       <c r="AP5" s="1"/>
       <c r="AQ5" s="1"/>
       <c r="AR5" s="1"/>
     </row>
     <row r="6" spans="1:47" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A6" s="69" t="s">
+      <c r="A6" s="215" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="70"/>
+      <c r="B6" s="216"/>
       <c r="C6" s="35"/>
-      <c r="D6" s="150" t="s">
+      <c r="D6" s="122" t="s">
         <v>80</v>
       </c>
-      <c r="E6" s="151"/>
-      <c r="F6" s="151"/>
-      <c r="G6" s="151"/>
-      <c r="H6" s="151"/>
-      <c r="I6" s="151"/>
-      <c r="J6" s="151"/>
-      <c r="K6" s="151"/>
-      <c r="L6" s="151"/>
-      <c r="M6" s="151"/>
-      <c r="N6" s="151"/>
-      <c r="O6" s="151"/>
-      <c r="P6" s="151"/>
-      <c r="Q6" s="151"/>
-      <c r="R6" s="151"/>
-      <c r="S6" s="151"/>
-      <c r="T6" s="151"/>
-      <c r="U6" s="151"/>
-      <c r="V6" s="151"/>
-      <c r="W6" s="151"/>
-      <c r="X6" s="151"/>
-      <c r="Y6" s="151"/>
-      <c r="Z6" s="151"/>
-      <c r="AA6" s="151"/>
-      <c r="AB6" s="151"/>
+      <c r="E6" s="123"/>
+      <c r="F6" s="123"/>
+      <c r="G6" s="123"/>
+      <c r="H6" s="123"/>
+      <c r="I6" s="123"/>
+      <c r="J6" s="123"/>
+      <c r="K6" s="123"/>
+      <c r="L6" s="123"/>
+      <c r="M6" s="123"/>
+      <c r="N6" s="123"/>
+      <c r="O6" s="123"/>
+      <c r="P6" s="123"/>
+      <c r="Q6" s="123"/>
+      <c r="R6" s="123"/>
+      <c r="S6" s="123"/>
+      <c r="T6" s="123"/>
+      <c r="U6" s="123"/>
+      <c r="V6" s="123"/>
+      <c r="W6" s="123"/>
+      <c r="X6" s="123"/>
+      <c r="Y6" s="123"/>
+      <c r="Z6" s="123"/>
+      <c r="AA6" s="123"/>
+      <c r="AB6" s="123"/>
       <c r="AC6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="AD6" s="152" t="s">
+      <c r="AD6" s="124" t="s">
         <v>18</v>
       </c>
-      <c r="AE6" s="153"/>
-      <c r="AF6" s="154" t="s">
+      <c r="AE6" s="125"/>
+      <c r="AF6" s="126" t="s">
         <v>19</v>
       </c>
-      <c r="AG6" s="155"/>
-      <c r="AH6" s="155"/>
-      <c r="AI6" s="155"/>
-      <c r="AJ6" s="155"/>
-      <c r="AK6" s="155"/>
-      <c r="AL6" s="155"/>
-      <c r="AM6" s="156"/>
+      <c r="AG6" s="127"/>
+      <c r="AH6" s="127"/>
+      <c r="AI6" s="127"/>
+      <c r="AJ6" s="127"/>
+      <c r="AK6" s="127"/>
+      <c r="AL6" s="127"/>
+      <c r="AM6" s="128"/>
       <c r="AN6" s="3"/>
       <c r="AO6" s="3"/>
       <c r="AP6" s="1"/>
@@ -3118,53 +3115,53 @@
       <c r="AR6" s="1"/>
     </row>
     <row r="7" spans="1:47" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="217" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="72"/>
+      <c r="B7" s="218"/>
       <c r="C7" s="34"/>
-      <c r="D7" s="157" t="s">
-        <v>81</v>
-      </c>
-      <c r="E7" s="158"/>
-      <c r="F7" s="158"/>
-      <c r="G7" s="158"/>
-      <c r="H7" s="158"/>
-      <c r="I7" s="158"/>
-      <c r="J7" s="158"/>
-      <c r="K7" s="158"/>
-      <c r="L7" s="158"/>
-      <c r="M7" s="158"/>
-      <c r="N7" s="158"/>
-      <c r="O7" s="158"/>
-      <c r="P7" s="158"/>
-      <c r="Q7" s="158"/>
-      <c r="R7" s="158"/>
+      <c r="D7" s="129" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="130"/>
+      <c r="F7" s="130"/>
+      <c r="G7" s="130"/>
+      <c r="H7" s="130"/>
+      <c r="I7" s="130"/>
+      <c r="J7" s="130"/>
+      <c r="K7" s="130"/>
+      <c r="L7" s="130"/>
+      <c r="M7" s="130"/>
+      <c r="N7" s="130"/>
+      <c r="O7" s="130"/>
+      <c r="P7" s="130"/>
+      <c r="Q7" s="130"/>
+      <c r="R7" s="130"/>
       <c r="S7" s="37"/>
-      <c r="T7" s="160" t="s">
+      <c r="T7" s="132" t="s">
         <v>21</v>
       </c>
-      <c r="U7" s="161"/>
-      <c r="V7" s="161"/>
-      <c r="W7" s="161"/>
-      <c r="X7" s="161"/>
-      <c r="Y7" s="161"/>
-      <c r="Z7" s="161"/>
-      <c r="AA7" s="161"/>
-      <c r="AB7" s="161"/>
-      <c r="AC7" s="161"/>
-      <c r="AD7" s="161"/>
-      <c r="AE7" s="161"/>
-      <c r="AF7" s="164" t="s">
+      <c r="U7" s="133"/>
+      <c r="V7" s="133"/>
+      <c r="W7" s="133"/>
+      <c r="X7" s="133"/>
+      <c r="Y7" s="133"/>
+      <c r="Z7" s="133"/>
+      <c r="AA7" s="133"/>
+      <c r="AB7" s="133"/>
+      <c r="AC7" s="133"/>
+      <c r="AD7" s="133"/>
+      <c r="AE7" s="133"/>
+      <c r="AF7" s="136" t="s">
         <v>22</v>
       </c>
-      <c r="AG7" s="165"/>
-      <c r="AH7" s="165"/>
-      <c r="AI7" s="166"/>
-      <c r="AJ7" s="166"/>
-      <c r="AK7" s="166"/>
-      <c r="AL7" s="166"/>
-      <c r="AM7" s="167"/>
+      <c r="AG7" s="137"/>
+      <c r="AH7" s="137"/>
+      <c r="AI7" s="138"/>
+      <c r="AJ7" s="138"/>
+      <c r="AK7" s="138"/>
+      <c r="AL7" s="138"/>
+      <c r="AM7" s="139"/>
       <c r="AN7" s="3"/>
       <c r="AO7" s="3"/>
       <c r="AP7" s="1"/>
@@ -3172,74 +3169,74 @@
       <c r="AR7" s="1"/>
     </row>
     <row r="8" spans="1:47" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="73"/>
-      <c r="B8" s="74"/>
+      <c r="A8" s="219"/>
+      <c r="B8" s="220"/>
       <c r="C8" s="36"/>
-      <c r="D8" s="159"/>
-      <c r="E8" s="159"/>
-      <c r="F8" s="159"/>
-      <c r="G8" s="159"/>
-      <c r="H8" s="159"/>
-      <c r="I8" s="159"/>
-      <c r="J8" s="159"/>
-      <c r="K8" s="158"/>
-      <c r="L8" s="158"/>
-      <c r="M8" s="158"/>
-      <c r="N8" s="158"/>
-      <c r="O8" s="158"/>
-      <c r="P8" s="158"/>
-      <c r="Q8" s="158"/>
-      <c r="R8" s="158"/>
+      <c r="D8" s="131"/>
+      <c r="E8" s="131"/>
+      <c r="F8" s="131"/>
+      <c r="G8" s="131"/>
+      <c r="H8" s="131"/>
+      <c r="I8" s="131"/>
+      <c r="J8" s="131"/>
+      <c r="K8" s="130"/>
+      <c r="L8" s="130"/>
+      <c r="M8" s="130"/>
+      <c r="N8" s="130"/>
+      <c r="O8" s="130"/>
+      <c r="P8" s="130"/>
+      <c r="Q8" s="130"/>
+      <c r="R8" s="130"/>
       <c r="S8" s="37"/>
-      <c r="T8" s="162"/>
-      <c r="U8" s="163"/>
-      <c r="V8" s="163"/>
-      <c r="W8" s="163"/>
-      <c r="X8" s="163"/>
-      <c r="Y8" s="163"/>
-      <c r="Z8" s="163"/>
-      <c r="AA8" s="163"/>
-      <c r="AB8" s="163"/>
-      <c r="AC8" s="163"/>
-      <c r="AD8" s="163"/>
-      <c r="AE8" s="163"/>
-      <c r="AF8" s="168" t="s">
+      <c r="T8" s="134"/>
+      <c r="U8" s="135"/>
+      <c r="V8" s="135"/>
+      <c r="W8" s="135"/>
+      <c r="X8" s="135"/>
+      <c r="Y8" s="135"/>
+      <c r="Z8" s="135"/>
+      <c r="AA8" s="135"/>
+      <c r="AB8" s="135"/>
+      <c r="AC8" s="135"/>
+      <c r="AD8" s="135"/>
+      <c r="AE8" s="135"/>
+      <c r="AF8" s="140" t="s">
         <v>23</v>
       </c>
-      <c r="AG8" s="169"/>
-      <c r="AH8" s="169"/>
-      <c r="AI8" s="169"/>
-      <c r="AJ8" s="169"/>
-      <c r="AK8" s="169"/>
-      <c r="AL8" s="169"/>
-      <c r="AM8" s="170"/>
+      <c r="AG8" s="141"/>
+      <c r="AH8" s="141"/>
+      <c r="AI8" s="141"/>
+      <c r="AJ8" s="141"/>
+      <c r="AK8" s="141"/>
+      <c r="AL8" s="141"/>
+      <c r="AM8" s="142"/>
       <c r="AN8" s="4"/>
       <c r="AO8" s="5"/>
-      <c r="AU8" s="247"/>
+      <c r="AU8" s="65"/>
     </row>
     <row r="9" spans="1:47" ht="43.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A9" s="177" t="s">
+      <c r="A9" s="149" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="178"/>
-      <c r="C9" s="178"/>
-      <c r="D9" s="178"/>
-      <c r="E9" s="178"/>
-      <c r="F9" s="183" t="s">
+      <c r="B9" s="150"/>
+      <c r="C9" s="150"/>
+      <c r="D9" s="150"/>
+      <c r="E9" s="150"/>
+      <c r="F9" s="155" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="183"/>
+      <c r="G9" s="155"/>
       <c r="H9" s="6" t="s">
         <v>25</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
-      <c r="K9" s="177" t="s">
+      <c r="K9" s="149" t="s">
         <v>26</v>
       </c>
-      <c r="L9" s="178"/>
-      <c r="M9" s="178"/>
-      <c r="N9" s="178"/>
+      <c r="L9" s="150"/>
+      <c r="M9" s="150"/>
+      <c r="N9" s="150"/>
       <c r="O9" s="9" t="s">
         <v>11</v>
       </c>
@@ -3249,52 +3246,56 @@
       <c r="Q9" s="6"/>
       <c r="R9" s="7"/>
       <c r="S9" s="8"/>
-      <c r="T9" s="248" t="s">
+      <c r="T9" s="114" t="s">
+        <v>85</v>
+      </c>
+      <c r="U9" s="117" t="s">
+        <v>86</v>
+      </c>
+      <c r="V9" s="117" t="s">
+        <v>87</v>
+      </c>
+      <c r="W9" s="117" t="s">
         <v>88</v>
       </c>
-      <c r="U9" s="251" t="s">
-        <v>89</v>
-      </c>
-      <c r="V9" s="251"/>
-      <c r="W9" s="251"/>
-      <c r="X9" s="251"/>
-      <c r="Y9" s="251"/>
-      <c r="Z9" s="251"/>
+      <c r="X9" s="117"/>
+      <c r="Y9" s="117"/>
+      <c r="Z9" s="117"/>
       <c r="AA9" s="61"/>
       <c r="AB9" s="61"/>
       <c r="AC9" s="61"/>
       <c r="AD9" s="61"/>
       <c r="AE9" s="61"/>
-      <c r="AF9" s="171"/>
-      <c r="AG9" s="172"/>
-      <c r="AH9" s="172"/>
-      <c r="AI9" s="172"/>
-      <c r="AJ9" s="172"/>
-      <c r="AK9" s="172"/>
-      <c r="AL9" s="172"/>
-      <c r="AM9" s="173"/>
+      <c r="AF9" s="143"/>
+      <c r="AG9" s="144"/>
+      <c r="AH9" s="144"/>
+      <c r="AI9" s="144"/>
+      <c r="AJ9" s="144"/>
+      <c r="AK9" s="144"/>
+      <c r="AL9" s="144"/>
+      <c r="AM9" s="145"/>
       <c r="AN9" s="5"/>
       <c r="AO9" s="5"/>
     </row>
     <row r="10" spans="1:47" ht="43.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A10" s="179"/>
-      <c r="B10" s="180"/>
-      <c r="C10" s="180"/>
-      <c r="D10" s="180"/>
-      <c r="E10" s="180"/>
-      <c r="F10" s="192" t="s">
+      <c r="A10" s="151"/>
+      <c r="B10" s="152"/>
+      <c r="C10" s="152"/>
+      <c r="D10" s="152"/>
+      <c r="E10" s="152"/>
+      <c r="F10" s="164" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="192"/>
+      <c r="G10" s="164"/>
       <c r="H10" s="38" t="s">
         <v>28</v>
       </c>
       <c r="I10" s="39"/>
       <c r="J10" s="39"/>
-      <c r="K10" s="179"/>
-      <c r="L10" s="180"/>
-      <c r="M10" s="180"/>
-      <c r="N10" s="180"/>
+      <c r="K10" s="151"/>
+      <c r="L10" s="152"/>
+      <c r="M10" s="152"/>
+      <c r="N10" s="152"/>
       <c r="O10" s="40" t="s">
         <v>6</v>
       </c>
@@ -3304,46 +3305,46 @@
       <c r="Q10" s="38"/>
       <c r="R10" s="39"/>
       <c r="S10" s="10"/>
-      <c r="T10" s="249"/>
-      <c r="U10" s="252"/>
-      <c r="V10" s="252"/>
-      <c r="W10" s="252"/>
-      <c r="X10" s="252"/>
-      <c r="Y10" s="252"/>
-      <c r="Z10" s="252"/>
+      <c r="T10" s="115"/>
+      <c r="U10" s="118"/>
+      <c r="V10" s="118"/>
+      <c r="W10" s="118"/>
+      <c r="X10" s="118"/>
+      <c r="Y10" s="118"/>
+      <c r="Z10" s="118"/>
       <c r="AA10" s="62"/>
       <c r="AB10" s="62"/>
       <c r="AC10" s="62"/>
       <c r="AD10" s="62"/>
       <c r="AE10" s="62"/>
-      <c r="AF10" s="171"/>
-      <c r="AG10" s="172"/>
-      <c r="AH10" s="172"/>
-      <c r="AI10" s="172"/>
-      <c r="AJ10" s="172"/>
-      <c r="AK10" s="172"/>
-      <c r="AL10" s="172"/>
-      <c r="AM10" s="173"/>
+      <c r="AF10" s="143"/>
+      <c r="AG10" s="144"/>
+      <c r="AH10" s="144"/>
+      <c r="AI10" s="144"/>
+      <c r="AJ10" s="144"/>
+      <c r="AK10" s="144"/>
+      <c r="AL10" s="144"/>
+      <c r="AM10" s="145"/>
       <c r="AN10" s="5"/>
       <c r="AO10" s="5"/>
     </row>
     <row r="11" spans="1:47" ht="43.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A11" s="179"/>
-      <c r="B11" s="180"/>
-      <c r="C11" s="180"/>
-      <c r="D11" s="180"/>
-      <c r="E11" s="180"/>
-      <c r="F11" s="193" t="s">
+      <c r="A11" s="151"/>
+      <c r="B11" s="152"/>
+      <c r="C11" s="152"/>
+      <c r="D11" s="152"/>
+      <c r="E11" s="152"/>
+      <c r="F11" s="165" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="193"/>
-      <c r="H11" s="194"/>
-      <c r="I11" s="194"/>
-      <c r="J11" s="194"/>
-      <c r="K11" s="179"/>
-      <c r="L11" s="180"/>
-      <c r="M11" s="180"/>
-      <c r="N11" s="180"/>
+      <c r="G11" s="165"/>
+      <c r="H11" s="166"/>
+      <c r="I11" s="166"/>
+      <c r="J11" s="166"/>
+      <c r="K11" s="151"/>
+      <c r="L11" s="152"/>
+      <c r="M11" s="152"/>
+      <c r="N11" s="152"/>
       <c r="O11" s="40" t="s">
         <v>6</v>
       </c>
@@ -3353,44 +3354,44 @@
       <c r="Q11" s="42"/>
       <c r="R11" s="39"/>
       <c r="S11" s="10"/>
-      <c r="T11" s="249"/>
-      <c r="U11" s="252"/>
-      <c r="V11" s="252"/>
-      <c r="W11" s="252"/>
-      <c r="X11" s="252"/>
-      <c r="Y11" s="252"/>
-      <c r="Z11" s="252"/>
+      <c r="T11" s="115"/>
+      <c r="U11" s="118"/>
+      <c r="V11" s="118"/>
+      <c r="W11" s="118"/>
+      <c r="X11" s="118"/>
+      <c r="Y11" s="118"/>
+      <c r="Z11" s="118"/>
       <c r="AA11" s="62"/>
       <c r="AB11" s="62"/>
       <c r="AC11" s="62"/>
       <c r="AD11" s="62"/>
       <c r="AE11" s="62"/>
-      <c r="AF11" s="171"/>
-      <c r="AG11" s="172"/>
-      <c r="AH11" s="172"/>
-      <c r="AI11" s="172"/>
-      <c r="AJ11" s="172"/>
-      <c r="AK11" s="172"/>
-      <c r="AL11" s="172"/>
-      <c r="AM11" s="173"/>
+      <c r="AF11" s="143"/>
+      <c r="AG11" s="144"/>
+      <c r="AH11" s="144"/>
+      <c r="AI11" s="144"/>
+      <c r="AJ11" s="144"/>
+      <c r="AK11" s="144"/>
+      <c r="AL11" s="144"/>
+      <c r="AM11" s="145"/>
     </row>
     <row r="12" spans="1:47" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A12" s="181"/>
-      <c r="B12" s="182"/>
-      <c r="C12" s="182"/>
-      <c r="D12" s="182"/>
-      <c r="E12" s="182"/>
-      <c r="F12" s="195" t="s">
+      <c r="A12" s="153"/>
+      <c r="B12" s="154"/>
+      <c r="C12" s="154"/>
+      <c r="D12" s="154"/>
+      <c r="E12" s="154"/>
+      <c r="F12" s="167" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="195"/>
-      <c r="H12" s="195"/>
-      <c r="I12" s="195"/>
-      <c r="J12" s="195"/>
-      <c r="K12" s="181"/>
-      <c r="L12" s="182"/>
-      <c r="M12" s="182"/>
-      <c r="N12" s="182"/>
+      <c r="G12" s="167"/>
+      <c r="H12" s="167"/>
+      <c r="I12" s="167"/>
+      <c r="J12" s="167"/>
+      <c r="K12" s="153"/>
+      <c r="L12" s="154"/>
+      <c r="M12" s="154"/>
+      <c r="N12" s="154"/>
       <c r="O12" s="11" t="s">
         <v>6</v>
       </c>
@@ -3400,320 +3401,320 @@
       <c r="Q12" s="13"/>
       <c r="R12" s="13"/>
       <c r="S12" s="14"/>
-      <c r="T12" s="249"/>
-      <c r="U12" s="252"/>
-      <c r="V12" s="252"/>
-      <c r="W12" s="252"/>
-      <c r="X12" s="252"/>
-      <c r="Y12" s="252"/>
-      <c r="Z12" s="252"/>
+      <c r="T12" s="115"/>
+      <c r="U12" s="118"/>
+      <c r="V12" s="118"/>
+      <c r="W12" s="118"/>
+      <c r="X12" s="118"/>
+      <c r="Y12" s="118"/>
+      <c r="Z12" s="118"/>
       <c r="AA12" s="62"/>
       <c r="AB12" s="62"/>
       <c r="AC12" s="62"/>
       <c r="AD12" s="62"/>
       <c r="AE12" s="62"/>
-      <c r="AF12" s="171"/>
-      <c r="AG12" s="172"/>
-      <c r="AH12" s="172"/>
-      <c r="AI12" s="172"/>
-      <c r="AJ12" s="172"/>
-      <c r="AK12" s="172"/>
-      <c r="AL12" s="172"/>
-      <c r="AM12" s="173"/>
+      <c r="AF12" s="143"/>
+      <c r="AG12" s="144"/>
+      <c r="AH12" s="144"/>
+      <c r="AI12" s="144"/>
+      <c r="AJ12" s="144"/>
+      <c r="AK12" s="144"/>
+      <c r="AL12" s="144"/>
+      <c r="AM12" s="145"/>
     </row>
     <row r="13" spans="1:47" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="184" t="s">
+      <c r="A13" s="156" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="185"/>
-      <c r="C13" s="185"/>
-      <c r="D13" s="185"/>
-      <c r="E13" s="185"/>
-      <c r="F13" s="185"/>
-      <c r="G13" s="185"/>
-      <c r="H13" s="185"/>
-      <c r="I13" s="185"/>
-      <c r="J13" s="185"/>
-      <c r="K13" s="186"/>
-      <c r="L13" s="186"/>
-      <c r="M13" s="186"/>
-      <c r="N13" s="186"/>
-      <c r="O13" s="186"/>
-      <c r="P13" s="186"/>
-      <c r="Q13" s="187"/>
-      <c r="R13" s="211" t="s">
+      <c r="B13" s="157"/>
+      <c r="C13" s="157"/>
+      <c r="D13" s="157"/>
+      <c r="E13" s="157"/>
+      <c r="F13" s="157"/>
+      <c r="G13" s="157"/>
+      <c r="H13" s="157"/>
+      <c r="I13" s="157"/>
+      <c r="J13" s="157"/>
+      <c r="K13" s="158"/>
+      <c r="L13" s="158"/>
+      <c r="M13" s="158"/>
+      <c r="N13" s="158"/>
+      <c r="O13" s="158"/>
+      <c r="P13" s="158"/>
+      <c r="Q13" s="159"/>
+      <c r="R13" s="108" t="s">
         <v>35</v>
       </c>
-      <c r="S13" s="212"/>
-      <c r="T13" s="249"/>
-      <c r="U13" s="252"/>
-      <c r="V13" s="252"/>
-      <c r="W13" s="252"/>
-      <c r="X13" s="252"/>
-      <c r="Y13" s="252"/>
-      <c r="Z13" s="252"/>
+      <c r="S13" s="109"/>
+      <c r="T13" s="115"/>
+      <c r="U13" s="118"/>
+      <c r="V13" s="118"/>
+      <c r="W13" s="118"/>
+      <c r="X13" s="118"/>
+      <c r="Y13" s="118"/>
+      <c r="Z13" s="118"/>
       <c r="AA13" s="62"/>
       <c r="AB13" s="62"/>
       <c r="AC13" s="62"/>
       <c r="AD13" s="62"/>
       <c r="AE13" s="62"/>
-      <c r="AF13" s="171"/>
-      <c r="AG13" s="172"/>
-      <c r="AH13" s="172"/>
-      <c r="AI13" s="172"/>
-      <c r="AJ13" s="172"/>
-      <c r="AK13" s="172"/>
-      <c r="AL13" s="172"/>
-      <c r="AM13" s="173"/>
+      <c r="AF13" s="143"/>
+      <c r="AG13" s="144"/>
+      <c r="AH13" s="144"/>
+      <c r="AI13" s="144"/>
+      <c r="AJ13" s="144"/>
+      <c r="AK13" s="144"/>
+      <c r="AL13" s="144"/>
+      <c r="AM13" s="145"/>
     </row>
     <row r="14" spans="1:47" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="188"/>
-      <c r="B14" s="186"/>
-      <c r="C14" s="186"/>
-      <c r="D14" s="186"/>
-      <c r="E14" s="186"/>
-      <c r="F14" s="186"/>
-      <c r="G14" s="186"/>
-      <c r="H14" s="186"/>
-      <c r="I14" s="186"/>
-      <c r="J14" s="186"/>
-      <c r="K14" s="186"/>
-      <c r="L14" s="186"/>
-      <c r="M14" s="186"/>
-      <c r="N14" s="186"/>
-      <c r="O14" s="186"/>
-      <c r="P14" s="186"/>
-      <c r="Q14" s="187"/>
-      <c r="R14" s="213"/>
-      <c r="S14" s="214"/>
-      <c r="T14" s="249"/>
-      <c r="U14" s="252"/>
-      <c r="V14" s="252"/>
-      <c r="W14" s="252"/>
-      <c r="X14" s="252"/>
-      <c r="Y14" s="252"/>
-      <c r="Z14" s="252"/>
+      <c r="A14" s="160"/>
+      <c r="B14" s="158"/>
+      <c r="C14" s="158"/>
+      <c r="D14" s="158"/>
+      <c r="E14" s="158"/>
+      <c r="F14" s="158"/>
+      <c r="G14" s="158"/>
+      <c r="H14" s="158"/>
+      <c r="I14" s="158"/>
+      <c r="J14" s="158"/>
+      <c r="K14" s="158"/>
+      <c r="L14" s="158"/>
+      <c r="M14" s="158"/>
+      <c r="N14" s="158"/>
+      <c r="O14" s="158"/>
+      <c r="P14" s="158"/>
+      <c r="Q14" s="159"/>
+      <c r="R14" s="110"/>
+      <c r="S14" s="111"/>
+      <c r="T14" s="115"/>
+      <c r="U14" s="118"/>
+      <c r="V14" s="118"/>
+      <c r="W14" s="118"/>
+      <c r="X14" s="118"/>
+      <c r="Y14" s="118"/>
+      <c r="Z14" s="118"/>
       <c r="AA14" s="62"/>
       <c r="AB14" s="62"/>
       <c r="AC14" s="62"/>
       <c r="AD14" s="62"/>
       <c r="AE14" s="62"/>
-      <c r="AF14" s="171"/>
-      <c r="AG14" s="172"/>
-      <c r="AH14" s="172"/>
-      <c r="AI14" s="172"/>
-      <c r="AJ14" s="172"/>
-      <c r="AK14" s="172"/>
-      <c r="AL14" s="172"/>
-      <c r="AM14" s="173"/>
+      <c r="AF14" s="143"/>
+      <c r="AG14" s="144"/>
+      <c r="AH14" s="144"/>
+      <c r="AI14" s="144"/>
+      <c r="AJ14" s="144"/>
+      <c r="AK14" s="144"/>
+      <c r="AL14" s="144"/>
+      <c r="AM14" s="145"/>
     </row>
     <row r="15" spans="1:47" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="188"/>
-      <c r="B15" s="186"/>
-      <c r="C15" s="186"/>
-      <c r="D15" s="186"/>
-      <c r="E15" s="186"/>
-      <c r="F15" s="186"/>
-      <c r="G15" s="186"/>
-      <c r="H15" s="186"/>
-      <c r="I15" s="186"/>
-      <c r="J15" s="186"/>
-      <c r="K15" s="186"/>
-      <c r="L15" s="186"/>
-      <c r="M15" s="186"/>
-      <c r="N15" s="186"/>
-      <c r="O15" s="186"/>
-      <c r="P15" s="186"/>
-      <c r="Q15" s="187"/>
-      <c r="R15" s="213"/>
-      <c r="S15" s="214"/>
-      <c r="T15" s="249"/>
-      <c r="U15" s="252"/>
-      <c r="V15" s="252"/>
-      <c r="W15" s="252"/>
-      <c r="X15" s="252"/>
-      <c r="Y15" s="252"/>
-      <c r="Z15" s="252"/>
+      <c r="A15" s="160"/>
+      <c r="B15" s="158"/>
+      <c r="C15" s="158"/>
+      <c r="D15" s="158"/>
+      <c r="E15" s="158"/>
+      <c r="F15" s="158"/>
+      <c r="G15" s="158"/>
+      <c r="H15" s="158"/>
+      <c r="I15" s="158"/>
+      <c r="J15" s="158"/>
+      <c r="K15" s="158"/>
+      <c r="L15" s="158"/>
+      <c r="M15" s="158"/>
+      <c r="N15" s="158"/>
+      <c r="O15" s="158"/>
+      <c r="P15" s="158"/>
+      <c r="Q15" s="159"/>
+      <c r="R15" s="110"/>
+      <c r="S15" s="111"/>
+      <c r="T15" s="115"/>
+      <c r="U15" s="118"/>
+      <c r="V15" s="118"/>
+      <c r="W15" s="118"/>
+      <c r="X15" s="118"/>
+      <c r="Y15" s="118"/>
+      <c r="Z15" s="118"/>
       <c r="AA15" s="62"/>
       <c r="AB15" s="62"/>
       <c r="AC15" s="62"/>
       <c r="AD15" s="62"/>
       <c r="AE15" s="62"/>
-      <c r="AF15" s="171"/>
-      <c r="AG15" s="172"/>
-      <c r="AH15" s="172"/>
-      <c r="AI15" s="172"/>
-      <c r="AJ15" s="172"/>
-      <c r="AK15" s="172"/>
-      <c r="AL15" s="172"/>
-      <c r="AM15" s="173"/>
+      <c r="AF15" s="143"/>
+      <c r="AG15" s="144"/>
+      <c r="AH15" s="144"/>
+      <c r="AI15" s="144"/>
+      <c r="AJ15" s="144"/>
+      <c r="AK15" s="144"/>
+      <c r="AL15" s="144"/>
+      <c r="AM15" s="145"/>
     </row>
     <row r="16" spans="1:47" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="189"/>
-      <c r="B16" s="190"/>
-      <c r="C16" s="190"/>
-      <c r="D16" s="190"/>
-      <c r="E16" s="190"/>
-      <c r="F16" s="190"/>
-      <c r="G16" s="190"/>
-      <c r="H16" s="190"/>
-      <c r="I16" s="190"/>
-      <c r="J16" s="190"/>
-      <c r="K16" s="190"/>
-      <c r="L16" s="190"/>
-      <c r="M16" s="190"/>
-      <c r="N16" s="190"/>
-      <c r="O16" s="190"/>
-      <c r="P16" s="190"/>
-      <c r="Q16" s="191"/>
-      <c r="R16" s="213"/>
-      <c r="S16" s="214"/>
-      <c r="T16" s="249"/>
-      <c r="U16" s="252"/>
-      <c r="V16" s="252"/>
-      <c r="W16" s="252"/>
-      <c r="X16" s="252"/>
-      <c r="Y16" s="252"/>
-      <c r="Z16" s="252"/>
+      <c r="A16" s="161"/>
+      <c r="B16" s="162"/>
+      <c r="C16" s="162"/>
+      <c r="D16" s="162"/>
+      <c r="E16" s="162"/>
+      <c r="F16" s="162"/>
+      <c r="G16" s="162"/>
+      <c r="H16" s="162"/>
+      <c r="I16" s="162"/>
+      <c r="J16" s="162"/>
+      <c r="K16" s="162"/>
+      <c r="L16" s="162"/>
+      <c r="M16" s="162"/>
+      <c r="N16" s="162"/>
+      <c r="O16" s="162"/>
+      <c r="P16" s="162"/>
+      <c r="Q16" s="163"/>
+      <c r="R16" s="110"/>
+      <c r="S16" s="111"/>
+      <c r="T16" s="115"/>
+      <c r="U16" s="118"/>
+      <c r="V16" s="118"/>
+      <c r="W16" s="118"/>
+      <c r="X16" s="118"/>
+      <c r="Y16" s="118"/>
+      <c r="Z16" s="118"/>
       <c r="AA16" s="62"/>
       <c r="AB16" s="62"/>
       <c r="AC16" s="62"/>
       <c r="AD16" s="62"/>
       <c r="AE16" s="62"/>
-      <c r="AF16" s="174"/>
-      <c r="AG16" s="175"/>
-      <c r="AH16" s="175"/>
-      <c r="AI16" s="175"/>
-      <c r="AJ16" s="175"/>
-      <c r="AK16" s="175"/>
-      <c r="AL16" s="175"/>
-      <c r="AM16" s="176"/>
+      <c r="AF16" s="146"/>
+      <c r="AG16" s="147"/>
+      <c r="AH16" s="147"/>
+      <c r="AI16" s="147"/>
+      <c r="AJ16" s="147"/>
+      <c r="AK16" s="147"/>
+      <c r="AL16" s="147"/>
+      <c r="AM16" s="148"/>
     </row>
     <row r="17" spans="1:39" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="80" t="s">
+      <c r="A17" s="226" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="82" t="s">
+      <c r="B17" s="228" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="83"/>
-      <c r="D17" s="83"/>
-      <c r="E17" s="83"/>
-      <c r="F17" s="83"/>
-      <c r="G17" s="83"/>
-      <c r="H17" s="83"/>
-      <c r="I17" s="83"/>
-      <c r="J17" s="83"/>
-      <c r="K17" s="88" t="s">
+      <c r="C17" s="229"/>
+      <c r="D17" s="229"/>
+      <c r="E17" s="229"/>
+      <c r="F17" s="229"/>
+      <c r="G17" s="229"/>
+      <c r="H17" s="229"/>
+      <c r="I17" s="229"/>
+      <c r="J17" s="229"/>
+      <c r="K17" s="234" t="s">
         <v>38</v>
       </c>
-      <c r="L17" s="89"/>
-      <c r="M17" s="82" t="s">
+      <c r="L17" s="235"/>
+      <c r="M17" s="228" t="s">
         <v>39</v>
       </c>
-      <c r="N17" s="83"/>
-      <c r="O17" s="83"/>
-      <c r="P17" s="94"/>
-      <c r="Q17" s="97" t="s">
+      <c r="N17" s="229"/>
+      <c r="O17" s="229"/>
+      <c r="P17" s="240"/>
+      <c r="Q17" s="243" t="s">
         <v>40</v>
       </c>
-      <c r="R17" s="213"/>
-      <c r="S17" s="214"/>
-      <c r="T17" s="249"/>
-      <c r="U17" s="252"/>
-      <c r="V17" s="252"/>
-      <c r="W17" s="252"/>
-      <c r="X17" s="252"/>
-      <c r="Y17" s="252"/>
-      <c r="Z17" s="252"/>
+      <c r="R17" s="110"/>
+      <c r="S17" s="111"/>
+      <c r="T17" s="115"/>
+      <c r="U17" s="118"/>
+      <c r="V17" s="118"/>
+      <c r="W17" s="118"/>
+      <c r="X17" s="118"/>
+      <c r="Y17" s="118"/>
+      <c r="Z17" s="118"/>
       <c r="AA17" s="62"/>
       <c r="AB17" s="62"/>
       <c r="AC17" s="62"/>
       <c r="AD17" s="62"/>
       <c r="AE17" s="62"/>
-      <c r="AF17" s="100" t="s">
+      <c r="AF17" s="246" t="s">
         <v>41</v>
       </c>
-      <c r="AG17" s="101"/>
-      <c r="AH17" s="100" t="s">
+      <c r="AG17" s="247"/>
+      <c r="AH17" s="246" t="s">
         <v>42</v>
       </c>
-      <c r="AI17" s="196"/>
-      <c r="AJ17" s="196"/>
-      <c r="AK17" s="196"/>
-      <c r="AL17" s="196"/>
-      <c r="AM17" s="197"/>
+      <c r="AI17" s="250"/>
+      <c r="AJ17" s="250"/>
+      <c r="AK17" s="250"/>
+      <c r="AL17" s="250"/>
+      <c r="AM17" s="251"/>
     </row>
     <row r="18" spans="1:39" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="81"/>
-      <c r="B18" s="84"/>
-      <c r="C18" s="85"/>
-      <c r="D18" s="85"/>
-      <c r="E18" s="85"/>
-      <c r="F18" s="85"/>
-      <c r="G18" s="85"/>
-      <c r="H18" s="85"/>
-      <c r="I18" s="85"/>
-      <c r="J18" s="85"/>
-      <c r="K18" s="90"/>
-      <c r="L18" s="91"/>
-      <c r="M18" s="84"/>
-      <c r="N18" s="85"/>
-      <c r="O18" s="85"/>
-      <c r="P18" s="95"/>
-      <c r="Q18" s="98"/>
-      <c r="R18" s="213"/>
-      <c r="S18" s="214"/>
-      <c r="T18" s="249"/>
-      <c r="U18" s="252"/>
-      <c r="V18" s="252"/>
-      <c r="W18" s="252"/>
-      <c r="X18" s="252"/>
-      <c r="Y18" s="252"/>
-      <c r="Z18" s="252"/>
+      <c r="A18" s="227"/>
+      <c r="B18" s="230"/>
+      <c r="C18" s="231"/>
+      <c r="D18" s="231"/>
+      <c r="E18" s="231"/>
+      <c r="F18" s="231"/>
+      <c r="G18" s="231"/>
+      <c r="H18" s="231"/>
+      <c r="I18" s="231"/>
+      <c r="J18" s="231"/>
+      <c r="K18" s="236"/>
+      <c r="L18" s="237"/>
+      <c r="M18" s="230"/>
+      <c r="N18" s="231"/>
+      <c r="O18" s="231"/>
+      <c r="P18" s="241"/>
+      <c r="Q18" s="244"/>
+      <c r="R18" s="110"/>
+      <c r="S18" s="111"/>
+      <c r="T18" s="115"/>
+      <c r="U18" s="118"/>
+      <c r="V18" s="118"/>
+      <c r="W18" s="118"/>
+      <c r="X18" s="118"/>
+      <c r="Y18" s="118"/>
+      <c r="Z18" s="118"/>
       <c r="AA18" s="62"/>
       <c r="AB18" s="62"/>
       <c r="AC18" s="62"/>
       <c r="AD18" s="62"/>
       <c r="AE18" s="62"/>
-      <c r="AF18" s="102"/>
-      <c r="AG18" s="103"/>
-      <c r="AH18" s="100"/>
-      <c r="AI18" s="196"/>
-      <c r="AJ18" s="196"/>
-      <c r="AK18" s="196"/>
-      <c r="AL18" s="196"/>
-      <c r="AM18" s="197"/>
+      <c r="AF18" s="248"/>
+      <c r="AG18" s="249"/>
+      <c r="AH18" s="246"/>
+      <c r="AI18" s="250"/>
+      <c r="AJ18" s="250"/>
+      <c r="AK18" s="250"/>
+      <c r="AL18" s="250"/>
+      <c r="AM18" s="251"/>
     </row>
     <row r="19" spans="1:39" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="86"/>
-      <c r="C19" s="87"/>
-      <c r="D19" s="87"/>
-      <c r="E19" s="87"/>
-      <c r="F19" s="87"/>
-      <c r="G19" s="87"/>
-      <c r="H19" s="87"/>
-      <c r="I19" s="87"/>
-      <c r="J19" s="87"/>
-      <c r="K19" s="92"/>
-      <c r="L19" s="93"/>
-      <c r="M19" s="86"/>
-      <c r="N19" s="87"/>
-      <c r="O19" s="87"/>
-      <c r="P19" s="96"/>
-      <c r="Q19" s="99"/>
-      <c r="R19" s="215"/>
-      <c r="S19" s="216"/>
-      <c r="T19" s="250"/>
-      <c r="U19" s="253"/>
-      <c r="V19" s="253"/>
-      <c r="W19" s="253"/>
-      <c r="X19" s="253"/>
-      <c r="Y19" s="253"/>
-      <c r="Z19" s="253"/>
+      <c r="B19" s="232"/>
+      <c r="C19" s="233"/>
+      <c r="D19" s="233"/>
+      <c r="E19" s="233"/>
+      <c r="F19" s="233"/>
+      <c r="G19" s="233"/>
+      <c r="H19" s="233"/>
+      <c r="I19" s="233"/>
+      <c r="J19" s="233"/>
+      <c r="K19" s="238"/>
+      <c r="L19" s="239"/>
+      <c r="M19" s="232"/>
+      <c r="N19" s="233"/>
+      <c r="O19" s="233"/>
+      <c r="P19" s="242"/>
+      <c r="Q19" s="245"/>
+      <c r="R19" s="112"/>
+      <c r="S19" s="113"/>
+      <c r="T19" s="116"/>
+      <c r="U19" s="119"/>
+      <c r="V19" s="119"/>
+      <c r="W19" s="119"/>
+      <c r="X19" s="119"/>
+      <c r="Y19" s="119"/>
+      <c r="Z19" s="119"/>
       <c r="AA19" s="63"/>
       <c r="AB19" s="63"/>
       <c r="AC19" s="63"/>
@@ -3725,45 +3726,45 @@
       <c r="AG19" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="AH19" s="102"/>
-      <c r="AI19" s="198"/>
-      <c r="AJ19" s="198"/>
-      <c r="AK19" s="198"/>
-      <c r="AL19" s="198"/>
-      <c r="AM19" s="199"/>
+      <c r="AH19" s="248"/>
+      <c r="AI19" s="252"/>
+      <c r="AJ19" s="252"/>
+      <c r="AK19" s="252"/>
+      <c r="AL19" s="252"/>
+      <c r="AM19" s="253"/>
     </row>
     <row r="20" spans="1:39" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A20" s="16"/>
-      <c r="B20" s="200" t="s">
-        <v>85</v>
-      </c>
-      <c r="C20" s="201"/>
-      <c r="D20" s="201"/>
-      <c r="E20" s="201"/>
-      <c r="F20" s="201"/>
-      <c r="G20" s="201"/>
-      <c r="H20" s="201"/>
-      <c r="I20" s="201"/>
-      <c r="J20" s="201"/>
-      <c r="K20" s="202" t="s">
-        <v>82</v>
-      </c>
-      <c r="L20" s="203"/>
-      <c r="M20" s="204"/>
-      <c r="N20" s="205"/>
-      <c r="O20" s="205"/>
-      <c r="P20" s="206"/>
+      <c r="B20" s="99"/>
+      <c r="C20" s="100"/>
+      <c r="D20" s="100"/>
+      <c r="E20" s="100"/>
+      <c r="F20" s="100"/>
+      <c r="G20" s="100"/>
+      <c r="H20" s="100"/>
+      <c r="I20" s="100"/>
+      <c r="J20" s="100"/>
+      <c r="K20" s="104" t="s">
+        <v>81</v>
+      </c>
+      <c r="L20" s="105"/>
+      <c r="M20" s="88"/>
+      <c r="N20" s="89"/>
+      <c r="O20" s="89"/>
+      <c r="P20" s="90"/>
       <c r="Q20" s="64">
         <v>2</v>
       </c>
-      <c r="R20" s="217" t="s">
-        <v>83</v>
-      </c>
-      <c r="S20" s="218"/>
+      <c r="R20" s="66" t="s">
+        <v>82</v>
+      </c>
+      <c r="S20" s="67"/>
       <c r="T20" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="U20" s="17"/>
+      <c r="U20" s="17" t="s">
+        <v>5</v>
+      </c>
       <c r="V20" s="17"/>
       <c r="W20" s="17"/>
       <c r="X20" s="17"/>
@@ -3780,47 +3781,43 @@
       <c r="AG20" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="AH20" s="207"/>
-      <c r="AI20" s="207"/>
-      <c r="AJ20" s="207"/>
-      <c r="AK20" s="207"/>
-      <c r="AL20" s="207"/>
-      <c r="AM20" s="208"/>
+      <c r="AH20" s="106"/>
+      <c r="AI20" s="106"/>
+      <c r="AJ20" s="106"/>
+      <c r="AK20" s="106"/>
+      <c r="AL20" s="106"/>
+      <c r="AM20" s="107"/>
     </row>
     <row r="21" spans="1:39" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A21" s="19"/>
-      <c r="B21" s="200" t="s">
-        <v>87</v>
-      </c>
-      <c r="C21" s="201"/>
-      <c r="D21" s="201"/>
-      <c r="E21" s="201"/>
-      <c r="F21" s="201"/>
-      <c r="G21" s="201"/>
-      <c r="H21" s="201"/>
-      <c r="I21" s="201"/>
-      <c r="J21" s="201"/>
-      <c r="K21" s="202" t="s">
-        <v>82</v>
-      </c>
-      <c r="L21" s="203"/>
-      <c r="M21" s="204"/>
-      <c r="N21" s="205"/>
-      <c r="O21" s="205"/>
-      <c r="P21" s="206"/>
-      <c r="Q21" s="64">
-        <v>1</v>
-      </c>
-      <c r="R21" s="217" t="s">
-        <v>84</v>
-      </c>
-      <c r="S21" s="218"/>
+      <c r="B21" s="99"/>
+      <c r="C21" s="100"/>
+      <c r="D21" s="100"/>
+      <c r="E21" s="100"/>
+      <c r="F21" s="100"/>
+      <c r="G21" s="100"/>
+      <c r="H21" s="100"/>
+      <c r="I21" s="100"/>
+      <c r="J21" s="100"/>
+      <c r="K21" s="104" t="s">
+        <v>81</v>
+      </c>
+      <c r="L21" s="105"/>
+      <c r="M21" s="88"/>
+      <c r="N21" s="89"/>
+      <c r="O21" s="89"/>
+      <c r="P21" s="90"/>
+      <c r="Q21" s="64"/>
+      <c r="R21" s="66"/>
+      <c r="S21" s="67"/>
       <c r="T21" s="20"/>
-      <c r="U21" s="20" t="s">
+      <c r="U21" s="20"/>
+      <c r="V21" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="V21" s="20"/>
-      <c r="W21" s="20"/>
+      <c r="W21" s="20" t="s">
+        <v>5</v>
+      </c>
       <c r="X21" s="20"/>
       <c r="Y21" s="20"/>
       <c r="Z21" s="20"/>
@@ -3835,34 +3832,35 @@
       <c r="AG21" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="AH21" s="209"/>
-      <c r="AI21" s="209"/>
-      <c r="AJ21" s="209"/>
-      <c r="AK21" s="209"/>
-      <c r="AL21" s="209"/>
-      <c r="AM21" s="210"/>
+      <c r="AH21" s="91"/>
+      <c r="AI21" s="91"/>
+      <c r="AJ21" s="91"/>
+      <c r="AK21" s="91"/>
+      <c r="AL21" s="91"/>
+      <c r="AM21" s="92"/>
     </row>
     <row r="22" spans="1:39" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A22" s="19"/>
-      <c r="B22" s="200"/>
-      <c r="C22" s="201"/>
-      <c r="D22" s="201"/>
-      <c r="E22" s="201"/>
-      <c r="F22" s="201"/>
-      <c r="G22" s="201"/>
-      <c r="H22" s="201"/>
-      <c r="I22" s="201"/>
-      <c r="J22" s="201"/>
-      <c r="K22" s="202"/>
-      <c r="L22" s="203"/>
-      <c r="M22" s="204"/>
-      <c r="N22" s="205"/>
-      <c r="O22" s="205"/>
-      <c r="P22" s="206"/>
+      <c r="B22" s="99"/>
+      <c r="C22" s="100"/>
+      <c r="D22" s="100"/>
+      <c r="E22" s="100"/>
+      <c r="F22" s="100"/>
+      <c r="G22" s="100"/>
+      <c r="H22" s="100"/>
+      <c r="I22" s="100"/>
+      <c r="J22" s="100"/>
+      <c r="K22" s="104"/>
+      <c r="L22" s="105"/>
+      <c r="M22" s="88"/>
+      <c r="N22" s="89"/>
+      <c r="O22" s="89"/>
+      <c r="P22" s="90"/>
       <c r="Q22" s="64"/>
-      <c r="R22" s="217"/>
-      <c r="S22" s="218"/>
+      <c r="R22" s="66"/>
+      <c r="S22" s="67"/>
       <c r="T22" s="20"/>
+      <c r="U22" s="20"/>
       <c r="V22" s="20"/>
       <c r="W22" s="20"/>
       <c r="X22" s="20"/>
@@ -3879,33 +3877,33 @@
       <c r="AG22" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="AH22" s="209"/>
-      <c r="AI22" s="209"/>
-      <c r="AJ22" s="209"/>
-      <c r="AK22" s="209"/>
-      <c r="AL22" s="209"/>
-      <c r="AM22" s="210"/>
+      <c r="AH22" s="91"/>
+      <c r="AI22" s="91"/>
+      <c r="AJ22" s="91"/>
+      <c r="AK22" s="91"/>
+      <c r="AL22" s="91"/>
+      <c r="AM22" s="92"/>
     </row>
     <row r="23" spans="1:39" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A23" s="19"/>
-      <c r="B23" s="200"/>
-      <c r="C23" s="201"/>
-      <c r="D23" s="201"/>
-      <c r="E23" s="201"/>
-      <c r="F23" s="201"/>
-      <c r="G23" s="201"/>
-      <c r="H23" s="201"/>
-      <c r="I23" s="201"/>
-      <c r="J23" s="201"/>
-      <c r="K23" s="202"/>
-      <c r="L23" s="203"/>
-      <c r="M23" s="204"/>
-      <c r="N23" s="205"/>
-      <c r="O23" s="205"/>
-      <c r="P23" s="206"/>
+      <c r="B23" s="99"/>
+      <c r="C23" s="100"/>
+      <c r="D23" s="100"/>
+      <c r="E23" s="100"/>
+      <c r="F23" s="100"/>
+      <c r="G23" s="100"/>
+      <c r="H23" s="100"/>
+      <c r="I23" s="100"/>
+      <c r="J23" s="100"/>
+      <c r="K23" s="104"/>
+      <c r="L23" s="105"/>
+      <c r="M23" s="88"/>
+      <c r="N23" s="89"/>
+      <c r="O23" s="89"/>
+      <c r="P23" s="90"/>
       <c r="Q23" s="64"/>
-      <c r="R23" s="217"/>
-      <c r="S23" s="218"/>
+      <c r="R23" s="66"/>
+      <c r="S23" s="67"/>
       <c r="T23" s="20"/>
       <c r="U23" s="20"/>
       <c r="V23" s="20"/>
@@ -3924,33 +3922,33 @@
       <c r="AG23" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="AH23" s="209"/>
-      <c r="AI23" s="209"/>
-      <c r="AJ23" s="209"/>
-      <c r="AK23" s="209"/>
-      <c r="AL23" s="209"/>
-      <c r="AM23" s="210"/>
+      <c r="AH23" s="91"/>
+      <c r="AI23" s="91"/>
+      <c r="AJ23" s="91"/>
+      <c r="AK23" s="91"/>
+      <c r="AL23" s="91"/>
+      <c r="AM23" s="92"/>
     </row>
     <row r="24" spans="1:39" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A24" s="19"/>
-      <c r="B24" s="200"/>
-      <c r="C24" s="201"/>
-      <c r="D24" s="201"/>
-      <c r="E24" s="201"/>
-      <c r="F24" s="201"/>
-      <c r="G24" s="201"/>
-      <c r="H24" s="201"/>
-      <c r="I24" s="201"/>
-      <c r="J24" s="201"/>
-      <c r="K24" s="202"/>
-      <c r="L24" s="203"/>
-      <c r="M24" s="204"/>
-      <c r="N24" s="205"/>
-      <c r="O24" s="205"/>
-      <c r="P24" s="206"/>
+      <c r="B24" s="99"/>
+      <c r="C24" s="100"/>
+      <c r="D24" s="100"/>
+      <c r="E24" s="100"/>
+      <c r="F24" s="100"/>
+      <c r="G24" s="100"/>
+      <c r="H24" s="100"/>
+      <c r="I24" s="100"/>
+      <c r="J24" s="100"/>
+      <c r="K24" s="104"/>
+      <c r="L24" s="105"/>
+      <c r="M24" s="88"/>
+      <c r="N24" s="89"/>
+      <c r="O24" s="89"/>
+      <c r="P24" s="90"/>
       <c r="Q24" s="64"/>
-      <c r="R24" s="217"/>
-      <c r="S24" s="218"/>
+      <c r="R24" s="66"/>
+      <c r="S24" s="67"/>
       <c r="T24" s="20"/>
       <c r="U24" s="20"/>
       <c r="V24" s="20"/>
@@ -3969,33 +3967,33 @@
       <c r="AG24" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="AH24" s="209"/>
-      <c r="AI24" s="209"/>
-      <c r="AJ24" s="209"/>
-      <c r="AK24" s="209"/>
-      <c r="AL24" s="209"/>
-      <c r="AM24" s="210"/>
+      <c r="AH24" s="91"/>
+      <c r="AI24" s="91"/>
+      <c r="AJ24" s="91"/>
+      <c r="AK24" s="91"/>
+      <c r="AL24" s="91"/>
+      <c r="AM24" s="92"/>
     </row>
     <row r="25" spans="1:39" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A25" s="19"/>
-      <c r="B25" s="200"/>
-      <c r="C25" s="201"/>
-      <c r="D25" s="201"/>
-      <c r="E25" s="201"/>
-      <c r="F25" s="201"/>
-      <c r="G25" s="201"/>
-      <c r="H25" s="201"/>
-      <c r="I25" s="201"/>
-      <c r="J25" s="201"/>
-      <c r="K25" s="202"/>
-      <c r="L25" s="203"/>
-      <c r="M25" s="204"/>
-      <c r="N25" s="205"/>
-      <c r="O25" s="205"/>
-      <c r="P25" s="206"/>
+      <c r="B25" s="99"/>
+      <c r="C25" s="100"/>
+      <c r="D25" s="100"/>
+      <c r="E25" s="100"/>
+      <c r="F25" s="100"/>
+      <c r="G25" s="100"/>
+      <c r="H25" s="100"/>
+      <c r="I25" s="100"/>
+      <c r="J25" s="100"/>
+      <c r="K25" s="104"/>
+      <c r="L25" s="105"/>
+      <c r="M25" s="88"/>
+      <c r="N25" s="89"/>
+      <c r="O25" s="89"/>
+      <c r="P25" s="90"/>
       <c r="Q25" s="64"/>
-      <c r="R25" s="217"/>
-      <c r="S25" s="218"/>
+      <c r="R25" s="66"/>
+      <c r="S25" s="67"/>
       <c r="T25" s="20"/>
       <c r="U25" s="20"/>
       <c r="V25" s="20"/>
@@ -4014,33 +4012,33 @@
       <c r="AG25" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="AH25" s="209"/>
-      <c r="AI25" s="209"/>
-      <c r="AJ25" s="209"/>
-      <c r="AK25" s="209"/>
-      <c r="AL25" s="209"/>
-      <c r="AM25" s="210"/>
+      <c r="AH25" s="91"/>
+      <c r="AI25" s="91"/>
+      <c r="AJ25" s="91"/>
+      <c r="AK25" s="91"/>
+      <c r="AL25" s="91"/>
+      <c r="AM25" s="92"/>
     </row>
     <row r="26" spans="1:39" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A26" s="19"/>
-      <c r="B26" s="200"/>
-      <c r="C26" s="201"/>
-      <c r="D26" s="201"/>
-      <c r="E26" s="201"/>
-      <c r="F26" s="201"/>
-      <c r="G26" s="201"/>
-      <c r="H26" s="201"/>
-      <c r="I26" s="201"/>
-      <c r="J26" s="201"/>
-      <c r="K26" s="202"/>
-      <c r="L26" s="203"/>
-      <c r="M26" s="204"/>
-      <c r="N26" s="205"/>
-      <c r="O26" s="205"/>
-      <c r="P26" s="206"/>
+      <c r="B26" s="99"/>
+      <c r="C26" s="100"/>
+      <c r="D26" s="100"/>
+      <c r="E26" s="100"/>
+      <c r="F26" s="100"/>
+      <c r="G26" s="100"/>
+      <c r="H26" s="100"/>
+      <c r="I26" s="100"/>
+      <c r="J26" s="100"/>
+      <c r="K26" s="104"/>
+      <c r="L26" s="105"/>
+      <c r="M26" s="88"/>
+      <c r="N26" s="89"/>
+      <c r="O26" s="89"/>
+      <c r="P26" s="90"/>
       <c r="Q26" s="64"/>
-      <c r="R26" s="217"/>
-      <c r="S26" s="218"/>
+      <c r="R26" s="66"/>
+      <c r="S26" s="67"/>
       <c r="T26" s="20"/>
       <c r="U26" s="20"/>
       <c r="V26" s="20"/>
@@ -4059,33 +4057,33 @@
       <c r="AG26" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="AH26" s="209"/>
-      <c r="AI26" s="209"/>
-      <c r="AJ26" s="209"/>
-      <c r="AK26" s="209"/>
-      <c r="AL26" s="209"/>
-      <c r="AM26" s="210"/>
+      <c r="AH26" s="91"/>
+      <c r="AI26" s="91"/>
+      <c r="AJ26" s="91"/>
+      <c r="AK26" s="91"/>
+      <c r="AL26" s="91"/>
+      <c r="AM26" s="92"/>
     </row>
     <row r="27" spans="1:39" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A27" s="19"/>
-      <c r="B27" s="200"/>
-      <c r="C27" s="201"/>
-      <c r="D27" s="201"/>
-      <c r="E27" s="201"/>
-      <c r="F27" s="201"/>
-      <c r="G27" s="201"/>
-      <c r="H27" s="201"/>
-      <c r="I27" s="201"/>
-      <c r="J27" s="201"/>
-      <c r="K27" s="202"/>
-      <c r="L27" s="203"/>
-      <c r="M27" s="204"/>
-      <c r="N27" s="205"/>
-      <c r="O27" s="205"/>
-      <c r="P27" s="206"/>
+      <c r="B27" s="99"/>
+      <c r="C27" s="100"/>
+      <c r="D27" s="100"/>
+      <c r="E27" s="100"/>
+      <c r="F27" s="100"/>
+      <c r="G27" s="100"/>
+      <c r="H27" s="100"/>
+      <c r="I27" s="100"/>
+      <c r="J27" s="100"/>
+      <c r="K27" s="104"/>
+      <c r="L27" s="105"/>
+      <c r="M27" s="88"/>
+      <c r="N27" s="89"/>
+      <c r="O27" s="89"/>
+      <c r="P27" s="90"/>
       <c r="Q27" s="64"/>
-      <c r="R27" s="217"/>
-      <c r="S27" s="218"/>
+      <c r="R27" s="66"/>
+      <c r="S27" s="67"/>
       <c r="T27" s="20"/>
       <c r="U27" s="20"/>
       <c r="V27" s="20"/>
@@ -4104,33 +4102,33 @@
       <c r="AG27" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="AH27" s="209"/>
-      <c r="AI27" s="209"/>
-      <c r="AJ27" s="209"/>
-      <c r="AK27" s="209"/>
-      <c r="AL27" s="209"/>
-      <c r="AM27" s="210"/>
+      <c r="AH27" s="91"/>
+      <c r="AI27" s="91"/>
+      <c r="AJ27" s="91"/>
+      <c r="AK27" s="91"/>
+      <c r="AL27" s="91"/>
+      <c r="AM27" s="92"/>
     </row>
     <row r="28" spans="1:39" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A28" s="19"/>
-      <c r="B28" s="200"/>
-      <c r="C28" s="201"/>
-      <c r="D28" s="201"/>
-      <c r="E28" s="201"/>
-      <c r="F28" s="201"/>
-      <c r="G28" s="201"/>
-      <c r="H28" s="201"/>
-      <c r="I28" s="201"/>
-      <c r="J28" s="201"/>
-      <c r="K28" s="202"/>
-      <c r="L28" s="203"/>
-      <c r="M28" s="204"/>
-      <c r="N28" s="205"/>
-      <c r="O28" s="205"/>
-      <c r="P28" s="206"/>
+      <c r="B28" s="99"/>
+      <c r="C28" s="100"/>
+      <c r="D28" s="100"/>
+      <c r="E28" s="100"/>
+      <c r="F28" s="100"/>
+      <c r="G28" s="100"/>
+      <c r="H28" s="100"/>
+      <c r="I28" s="100"/>
+      <c r="J28" s="100"/>
+      <c r="K28" s="104"/>
+      <c r="L28" s="105"/>
+      <c r="M28" s="88"/>
+      <c r="N28" s="89"/>
+      <c r="O28" s="89"/>
+      <c r="P28" s="90"/>
       <c r="Q28" s="64"/>
-      <c r="R28" s="217"/>
-      <c r="S28" s="218"/>
+      <c r="R28" s="66"/>
+      <c r="S28" s="67"/>
       <c r="T28" s="20"/>
       <c r="U28" s="20"/>
       <c r="V28" s="20"/>
@@ -4149,33 +4147,33 @@
       <c r="AG28" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="AH28" s="209"/>
-      <c r="AI28" s="209"/>
-      <c r="AJ28" s="209"/>
-      <c r="AK28" s="209"/>
-      <c r="AL28" s="209"/>
-      <c r="AM28" s="210"/>
+      <c r="AH28" s="91"/>
+      <c r="AI28" s="91"/>
+      <c r="AJ28" s="91"/>
+      <c r="AK28" s="91"/>
+      <c r="AL28" s="91"/>
+      <c r="AM28" s="92"/>
     </row>
     <row r="29" spans="1:39" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
       <c r="A29" s="22"/>
-      <c r="B29" s="200"/>
-      <c r="C29" s="201"/>
-      <c r="D29" s="201"/>
-      <c r="E29" s="201"/>
-      <c r="F29" s="201"/>
-      <c r="G29" s="201"/>
-      <c r="H29" s="201"/>
-      <c r="I29" s="201"/>
-      <c r="J29" s="201"/>
-      <c r="K29" s="202"/>
-      <c r="L29" s="203"/>
-      <c r="M29" s="204"/>
-      <c r="N29" s="205"/>
-      <c r="O29" s="205"/>
-      <c r="P29" s="206"/>
+      <c r="B29" s="99"/>
+      <c r="C29" s="100"/>
+      <c r="D29" s="100"/>
+      <c r="E29" s="100"/>
+      <c r="F29" s="100"/>
+      <c r="G29" s="100"/>
+      <c r="H29" s="100"/>
+      <c r="I29" s="100"/>
+      <c r="J29" s="100"/>
+      <c r="K29" s="104"/>
+      <c r="L29" s="105"/>
+      <c r="M29" s="88"/>
+      <c r="N29" s="89"/>
+      <c r="O29" s="89"/>
+      <c r="P29" s="90"/>
       <c r="Q29" s="64"/>
-      <c r="R29" s="217"/>
-      <c r="S29" s="218"/>
+      <c r="R29" s="66"/>
+      <c r="S29" s="67"/>
       <c r="T29" s="23"/>
       <c r="U29" s="23"/>
       <c r="V29" s="23"/>
@@ -4194,59 +4192,59 @@
       <c r="AG29" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="AH29" s="245"/>
-      <c r="AI29" s="245"/>
-      <c r="AJ29" s="245"/>
-      <c r="AK29" s="245"/>
-      <c r="AL29" s="245"/>
-      <c r="AM29" s="246"/>
+      <c r="AH29" s="93"/>
+      <c r="AI29" s="93"/>
+      <c r="AJ29" s="93"/>
+      <c r="AK29" s="93"/>
+      <c r="AL29" s="93"/>
+      <c r="AM29" s="94"/>
     </row>
     <row r="30" spans="1:39" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="219" t="s">
+      <c r="A30" s="78" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="219" t="s">
+      <c r="B30" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="220"/>
-      <c r="D30" s="220" t="s">
+      <c r="C30" s="72"/>
+      <c r="D30" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="E30" s="220"/>
+      <c r="E30" s="72"/>
       <c r="F30" s="60"/>
-      <c r="G30" s="220" t="s">
+      <c r="G30" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="H30" s="220"/>
+      <c r="H30" s="72"/>
       <c r="I30" s="60"/>
-      <c r="J30" s="225" t="s">
+      <c r="J30" s="97" t="s">
         <v>50</v>
       </c>
-      <c r="K30" s="223" t="s">
+      <c r="K30" s="95" t="s">
         <v>51</v>
       </c>
-      <c r="L30" s="234" t="s">
+      <c r="L30" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="M30" s="234"/>
-      <c r="N30" s="234" t="s">
+      <c r="M30" s="74"/>
+      <c r="N30" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="O30" s="234"/>
-      <c r="P30" s="234" t="s">
+      <c r="O30" s="74"/>
+      <c r="P30" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="Q30" s="236"/>
-      <c r="R30" s="219" t="s">
+      <c r="Q30" s="76"/>
+      <c r="R30" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="S30" s="220"/>
-      <c r="T30" s="238" t="s">
+      <c r="S30" s="72"/>
+      <c r="T30" s="81" t="s">
         <v>54</v>
       </c>
-      <c r="U30" s="238"/>
-      <c r="V30" s="238"/>
-      <c r="W30" s="239"/>
+      <c r="U30" s="81"/>
+      <c r="V30" s="81"/>
+      <c r="W30" s="82"/>
       <c r="X30" s="51" t="s">
         <v>55</v>
       </c>
@@ -4265,51 +4263,51 @@
       <c r="AE30" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="AF30" s="242" t="s">
+      <c r="AF30" s="85" t="s">
         <v>59</v>
       </c>
-      <c r="AG30" s="243"/>
-      <c r="AH30" s="220" t="s">
+      <c r="AG30" s="86"/>
+      <c r="AH30" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="AI30" s="220"/>
-      <c r="AJ30" s="220" t="s">
+      <c r="AI30" s="72"/>
+      <c r="AJ30" s="72" t="s">
         <v>61</v>
       </c>
-      <c r="AK30" s="220"/>
-      <c r="AL30" s="230" t="s">
+      <c r="AK30" s="72"/>
+      <c r="AL30" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="AM30" s="231"/>
+      <c r="AM30" s="69"/>
     </row>
     <row r="31" spans="1:39" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="221"/>
-      <c r="B31" s="221"/>
-      <c r="C31" s="222"/>
-      <c r="D31" s="227" t="s">
+      <c r="A31" s="79"/>
+      <c r="B31" s="79"/>
+      <c r="C31" s="80"/>
+      <c r="D31" s="98" t="s">
         <v>63</v>
       </c>
-      <c r="E31" s="227"/>
-      <c r="F31" s="227"/>
-      <c r="G31" s="227" t="s">
+      <c r="E31" s="98"/>
+      <c r="F31" s="98"/>
+      <c r="G31" s="98" t="s">
         <v>64</v>
       </c>
-      <c r="H31" s="227"/>
-      <c r="I31" s="227"/>
-      <c r="J31" s="226"/>
-      <c r="K31" s="224"/>
-      <c r="L31" s="235"/>
-      <c r="M31" s="235"/>
-      <c r="N31" s="235"/>
-      <c r="O31" s="235"/>
-      <c r="P31" s="235"/>
-      <c r="Q31" s="237"/>
-      <c r="R31" s="221"/>
-      <c r="S31" s="222"/>
-      <c r="T31" s="240"/>
-      <c r="U31" s="240"/>
-      <c r="V31" s="240"/>
-      <c r="W31" s="241"/>
+      <c r="H31" s="98"/>
+      <c r="I31" s="98"/>
+      <c r="J31" s="71"/>
+      <c r="K31" s="96"/>
+      <c r="L31" s="75"/>
+      <c r="M31" s="75"/>
+      <c r="N31" s="75"/>
+      <c r="O31" s="75"/>
+      <c r="P31" s="75"/>
+      <c r="Q31" s="77"/>
+      <c r="R31" s="79"/>
+      <c r="S31" s="80"/>
+      <c r="T31" s="83"/>
+      <c r="U31" s="83"/>
+      <c r="V31" s="83"/>
+      <c r="W31" s="84"/>
       <c r="X31" s="56" t="s">
         <v>65</v>
       </c>
@@ -4324,127 +4322,245 @@
         <v>66</v>
       </c>
       <c r="AG31" s="57"/>
-      <c r="AH31" s="233" t="s">
+      <c r="AH31" s="73" t="s">
         <v>67</v>
       </c>
-      <c r="AI31" s="233"/>
-      <c r="AJ31" s="244" t="s">
+      <c r="AI31" s="73"/>
+      <c r="AJ31" s="87" t="s">
         <v>67</v>
       </c>
-      <c r="AK31" s="244"/>
-      <c r="AL31" s="232" t="s">
+      <c r="AK31" s="87"/>
+      <c r="AL31" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="AM31" s="226"/>
+      <c r="AM31" s="71"/>
     </row>
     <row r="32" spans="1:39" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="25" t="s">
         <v>68</v>
       </c>
       <c r="B32" s="26"/>
-      <c r="C32" s="75"/>
-      <c r="D32" s="75"/>
-      <c r="E32" s="75"/>
-      <c r="F32" s="75"/>
-      <c r="G32" s="75"/>
-      <c r="H32" s="75"/>
+      <c r="C32" s="221"/>
+      <c r="D32" s="221"/>
+      <c r="E32" s="221"/>
+      <c r="F32" s="221"/>
+      <c r="G32" s="221"/>
+      <c r="H32" s="221"/>
       <c r="I32" s="26" t="s">
         <v>69</v>
       </c>
       <c r="J32" s="26"/>
-      <c r="K32" s="77"/>
-      <c r="L32" s="77"/>
-      <c r="M32" s="77"/>
-      <c r="N32" s="77"/>
-      <c r="O32" s="77"/>
+      <c r="K32" s="223"/>
+      <c r="L32" s="223"/>
+      <c r="M32" s="223"/>
+      <c r="N32" s="223"/>
+      <c r="O32" s="223"/>
       <c r="P32" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="Q32" s="77"/>
-      <c r="R32" s="77"/>
-      <c r="S32" s="77"/>
-      <c r="T32" s="78"/>
+      <c r="Q32" s="223"/>
+      <c r="R32" s="223"/>
+      <c r="S32" s="223"/>
+      <c r="T32" s="224"/>
       <c r="U32" s="48" t="s">
         <v>71</v>
       </c>
       <c r="V32" s="47"/>
-      <c r="W32" s="77"/>
-      <c r="X32" s="75"/>
-      <c r="Y32" s="75"/>
-      <c r="Z32" s="75"/>
-      <c r="AA32" s="75"/>
+      <c r="W32" s="223"/>
+      <c r="X32" s="221"/>
+      <c r="Y32" s="221"/>
+      <c r="Z32" s="221"/>
+      <c r="AA32" s="221"/>
       <c r="AB32" s="26" t="s">
         <v>72</v>
       </c>
       <c r="AC32" s="28"/>
-      <c r="AD32" s="65"/>
-      <c r="AE32" s="65"/>
-      <c r="AF32" s="65"/>
-      <c r="AG32" s="65"/>
-      <c r="AH32" s="65"/>
+      <c r="AD32" s="211"/>
+      <c r="AE32" s="211"/>
+      <c r="AF32" s="211"/>
+      <c r="AG32" s="211"/>
+      <c r="AH32" s="211"/>
       <c r="AI32" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="AJ32" s="65"/>
-      <c r="AK32" s="65"/>
-      <c r="AL32" s="65"/>
-      <c r="AM32" s="66"/>
+      <c r="AJ32" s="211"/>
+      <c r="AK32" s="211"/>
+      <c r="AL32" s="211"/>
+      <c r="AM32" s="212"/>
     </row>
     <row r="33" spans="1:39" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="33" t="s">
         <v>68</v>
       </c>
       <c r="B33" s="29"/>
-      <c r="C33" s="76"/>
-      <c r="D33" s="76"/>
-      <c r="E33" s="76"/>
-      <c r="F33" s="76"/>
-      <c r="G33" s="76"/>
-      <c r="H33" s="76"/>
+      <c r="C33" s="222"/>
+      <c r="D33" s="222"/>
+      <c r="E33" s="222"/>
+      <c r="F33" s="222"/>
+      <c r="G33" s="222"/>
+      <c r="H33" s="222"/>
       <c r="I33" s="29" t="s">
         <v>69</v>
       </c>
       <c r="J33" s="29"/>
-      <c r="K33" s="76"/>
-      <c r="L33" s="76"/>
-      <c r="M33" s="76"/>
-      <c r="N33" s="76"/>
-      <c r="O33" s="76"/>
+      <c r="K33" s="222"/>
+      <c r="L33" s="222"/>
+      <c r="M33" s="222"/>
+      <c r="N33" s="222"/>
+      <c r="O33" s="222"/>
       <c r="P33" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="Q33" s="76"/>
-      <c r="R33" s="76"/>
-      <c r="S33" s="76"/>
-      <c r="T33" s="79"/>
+      <c r="Q33" s="222"/>
+      <c r="R33" s="222"/>
+      <c r="S33" s="222"/>
+      <c r="T33" s="225"/>
       <c r="U33" s="29" t="s">
         <v>71</v>
       </c>
       <c r="V33" s="30"/>
-      <c r="W33" s="76"/>
-      <c r="X33" s="76"/>
-      <c r="Y33" s="76"/>
-      <c r="Z33" s="76"/>
-      <c r="AA33" s="76"/>
+      <c r="W33" s="222"/>
+      <c r="X33" s="222"/>
+      <c r="Y33" s="222"/>
+      <c r="Z33" s="222"/>
+      <c r="AA33" s="222"/>
       <c r="AB33" s="29" t="s">
         <v>72</v>
       </c>
       <c r="AC33" s="31"/>
-      <c r="AD33" s="67"/>
-      <c r="AE33" s="67"/>
-      <c r="AF33" s="67"/>
-      <c r="AG33" s="67"/>
-      <c r="AH33" s="67"/>
+      <c r="AD33" s="213"/>
+      <c r="AE33" s="213"/>
+      <c r="AF33" s="213"/>
+      <c r="AG33" s="213"/>
+      <c r="AH33" s="213"/>
       <c r="AI33" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="AJ33" s="67"/>
-      <c r="AK33" s="67"/>
-      <c r="AL33" s="67"/>
-      <c r="AM33" s="68"/>
+      <c r="AJ33" s="213"/>
+      <c r="AK33" s="213"/>
+      <c r="AL33" s="213"/>
+      <c r="AM33" s="214"/>
     </row>
   </sheetData>
   <mergeCells count="143">
+    <mergeCell ref="AJ32:AM32"/>
+    <mergeCell ref="AJ33:AM33"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B8"/>
+    <mergeCell ref="C32:H32"/>
+    <mergeCell ref="C33:H33"/>
+    <mergeCell ref="K32:O32"/>
+    <mergeCell ref="K33:O33"/>
+    <mergeCell ref="Q32:T32"/>
+    <mergeCell ref="Q33:T33"/>
+    <mergeCell ref="W32:AA32"/>
+    <mergeCell ref="W33:AA33"/>
+    <mergeCell ref="AD32:AH32"/>
+    <mergeCell ref="AD33:AH33"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:J19"/>
+    <mergeCell ref="K17:L19"/>
+    <mergeCell ref="M17:P19"/>
+    <mergeCell ref="Q17:Q19"/>
+    <mergeCell ref="AF17:AG18"/>
+    <mergeCell ref="AH17:AM19"/>
+    <mergeCell ref="B20:J20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="M20:P20"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="J1:AE1"/>
+    <mergeCell ref="AF1:AI2"/>
+    <mergeCell ref="AJ1:AM5"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:AE2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:U3"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="X3:AE3"/>
+    <mergeCell ref="AF3:AI3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="L4:U4"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="X4:AE4"/>
+    <mergeCell ref="AF4:AI5"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:U5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="X5:AE5"/>
+    <mergeCell ref="D6:AB6"/>
+    <mergeCell ref="AD6:AE6"/>
+    <mergeCell ref="AF6:AM6"/>
+    <mergeCell ref="D7:R8"/>
+    <mergeCell ref="T7:AE8"/>
+    <mergeCell ref="AF7:AH7"/>
+    <mergeCell ref="AI7:AM7"/>
+    <mergeCell ref="AF8:AM16"/>
+    <mergeCell ref="A9:E12"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="K9:N12"/>
+    <mergeCell ref="A13:Q16"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="AH20:AM20"/>
+    <mergeCell ref="B21:J21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="M21:P21"/>
+    <mergeCell ref="AH21:AM21"/>
+    <mergeCell ref="R13:S19"/>
+    <mergeCell ref="R20:S20"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="T9:T19"/>
+    <mergeCell ref="U9:U19"/>
+    <mergeCell ref="V9:V19"/>
+    <mergeCell ref="W9:W19"/>
+    <mergeCell ref="X9:X19"/>
+    <mergeCell ref="Y9:Y19"/>
+    <mergeCell ref="Z9:Z19"/>
+    <mergeCell ref="M24:P24"/>
+    <mergeCell ref="AH24:AM24"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:P25"/>
+    <mergeCell ref="AH25:AM25"/>
+    <mergeCell ref="B22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M22:P22"/>
+    <mergeCell ref="AH22:AM22"/>
+    <mergeCell ref="B23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="M23:P23"/>
+    <mergeCell ref="AH23:AM23"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="R24:S24"/>
+    <mergeCell ref="R25:S25"/>
+    <mergeCell ref="C2:I2"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="B28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="B29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="B26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="B24:J24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="B30:C31"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="G30:H30"/>
     <mergeCell ref="B27:J27"/>
     <mergeCell ref="R26:S26"/>
     <mergeCell ref="R27:S27"/>
@@ -4470,136 +4586,18 @@
     <mergeCell ref="AH26:AM26"/>
     <mergeCell ref="M27:P27"/>
     <mergeCell ref="AH27:AM27"/>
-    <mergeCell ref="B30:C31"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="C2:I2"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="B28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="B29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="B26:J26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="B24:J24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="M24:P24"/>
-    <mergeCell ref="AH24:AM24"/>
-    <mergeCell ref="B25:J25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M25:P25"/>
-    <mergeCell ref="AH25:AM25"/>
-    <mergeCell ref="B22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="M22:P22"/>
-    <mergeCell ref="AH22:AM22"/>
-    <mergeCell ref="B23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="M23:P23"/>
-    <mergeCell ref="AH23:AM23"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="R24:S24"/>
-    <mergeCell ref="R25:S25"/>
-    <mergeCell ref="AH17:AM19"/>
-    <mergeCell ref="B20:J20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="M20:P20"/>
-    <mergeCell ref="AH20:AM20"/>
-    <mergeCell ref="B21:J21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="M21:P21"/>
-    <mergeCell ref="AH21:AM21"/>
-    <mergeCell ref="R13:S19"/>
-    <mergeCell ref="R20:S20"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="T9:T19"/>
-    <mergeCell ref="U9:U19"/>
-    <mergeCell ref="V9:V19"/>
-    <mergeCell ref="W9:W19"/>
-    <mergeCell ref="X9:X19"/>
-    <mergeCell ref="Y9:Y19"/>
-    <mergeCell ref="Z9:Z19"/>
-    <mergeCell ref="X5:AE5"/>
-    <mergeCell ref="D6:AB6"/>
-    <mergeCell ref="AD6:AE6"/>
-    <mergeCell ref="AF6:AM6"/>
-    <mergeCell ref="D7:R8"/>
-    <mergeCell ref="T7:AE8"/>
-    <mergeCell ref="AF7:AH7"/>
-    <mergeCell ref="AI7:AM7"/>
-    <mergeCell ref="AF8:AM16"/>
-    <mergeCell ref="A9:E12"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="K9:N12"/>
-    <mergeCell ref="A13:Q16"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="F12:J12"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="J1:AE1"/>
-    <mergeCell ref="AF1:AI2"/>
-    <mergeCell ref="AJ1:AM5"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:AE2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:U3"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="X3:AE3"/>
-    <mergeCell ref="AF3:AI3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="L4:U4"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="X4:AE4"/>
-    <mergeCell ref="AF4:AI5"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:U5"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="AJ32:AM32"/>
-    <mergeCell ref="AJ33:AM33"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B8"/>
-    <mergeCell ref="C32:H32"/>
-    <mergeCell ref="C33:H33"/>
-    <mergeCell ref="K32:O32"/>
-    <mergeCell ref="K33:O33"/>
-    <mergeCell ref="Q32:T32"/>
-    <mergeCell ref="Q33:T33"/>
-    <mergeCell ref="W32:AA32"/>
-    <mergeCell ref="W33:AA33"/>
-    <mergeCell ref="AD32:AH32"/>
-    <mergeCell ref="AD33:AH33"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:J19"/>
-    <mergeCell ref="K17:L19"/>
-    <mergeCell ref="M17:P19"/>
-    <mergeCell ref="Q17:Q19"/>
-    <mergeCell ref="AF17:AG18"/>
   </mergeCells>
   <phoneticPr fontId="36" type="noConversion"/>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="CoC Check boxes" prompt="Mark box by selecting X from the drop down list" sqref="F9:G10 O9:O12 AC6" xr:uid="{6B25F282-0C23-4D59-8943-01577D0F6E13}">
       <formula1>$AP$2:$AP$3</formula1>
     </dataValidation>
+    <dataValidation showErrorMessage="1" promptTitle="Analysis Check Box" prompt="Select X from drop down menu to mark this field for analysis." sqref="Y30:AE31 T30" xr:uid="{CC78C49A-0914-451A-AF70-A4D3FA8E66A2}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="CoC Check Boxes" prompt="Select X from the drop down menu to mark this field." sqref="AF30:AG31" xr:uid="{CAA851DD-850A-46CE-B54F-68FFD9F331CC}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="CoC Check Boxes" prompt="Select X from the drop down menu to mark this field." sqref="AF20:AG29" xr:uid="{EF49C837-A4F2-4BEC-A69A-9A897971FB61}">
       <formula1>$AP$2:$AP$3</formula1>
     </dataValidation>
-    <dataValidation showErrorMessage="1" promptTitle="Analysis Check Box" prompt="Select X from drop down menu to mark this field for analysis." sqref="Y30:AE31 T30" xr:uid="{CC78C49A-0914-451A-AF70-A4D3FA8E66A2}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="CoC Check Boxes" prompt="Select X from the drop down menu to mark this field." sqref="AF30:AG31" xr:uid="{CAA851DD-850A-46CE-B54F-68FFD9F331CC}"/>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Analysis Check Box" prompt="Select X from drop down menu to mark this field for analysis." sqref="T22 T20:AE21 V22:AE22 T23:AE29" xr:uid="{D5413070-99C9-4D9F-A9B0-EF2A7BE67091}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Analysis Check Box" prompt="Select X from drop down menu to mark this field for analysis." sqref="T20:AE29" xr:uid="{D5413070-99C9-4D9F-A9B0-EF2A7BE67091}">
       <formula1>$AO$2:$AO$2</formula1>
     </dataValidation>
   </dataValidations>
@@ -4609,7 +4607,7 @@
   </hyperlinks>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.35433070866141736" bottom="0.26250000000000001" header="0" footer="0.10062500000000001"/>
-  <pageSetup paperSize="9" scale="42" orientation="landscape" r:id="rId3"/>
+  <pageSetup paperSize="9" scale="41" orientation="landscape" r:id="rId3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;L&amp;"Avenir Next LT Pro,Regular" ENFM (204/17)&amp;C&amp;"Avenir Next LT Pro,Regular"Form Page 1 of 1&amp;R&amp;"Avenir Next LT Pro,Regular"Approved Date: 13/02/2024                    </oddFooter>
   </headerFooter>
@@ -4618,8 +4616,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007846347A7CE9C4479D532F5E79B2E425" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="03af9fba1cc086f23fc2ecca9f20b105">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="55afd7b3-9a07-47b7-a1cd-476572e086a0" xmlns:ns3="3e405550-e584-4020-9399-da0f1982afa1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="490eb9187725e31a73776e23b63e4463" ns1:_="" ns2:_="" ns3:_="">
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007846347A7CE9C4479D532F5E79B2E425" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="48c3045064959f25dff2ce4f240aeb4c">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="55afd7b3-9a07-47b7-a1cd-476572e086a0" xmlns:ns3="3e405550-e584-4020-9399-da0f1982afa1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="48b8bd9fee98862fbb4b2635dce8ffdf" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="55afd7b3-9a07-47b7-a1cd-476572e086a0"/>
     <xsd:import namespace="3e405550-e584-4020-9399-da0f1982afa1"/>
@@ -4899,15 +4906,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4924,7 +4922,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8D5BC5D-A610-446C-A89C-B091DB8C0EA4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96C5C6E1-8D52-49B3-AC15-E0A50311643F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08AD828F-53A1-4F4E-BF89-0FA350809583}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -4939,14 +4945,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96C5C6E1-8D52-49B3-AC15-E0A50311643F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>